<commit_message>
24/05/2023 update. SonarLint issues fixed.
</commit_message>
<xml_diff>
--- a/src/main/resources/static/companies.xlsx
+++ b/src/main/resources/static/companies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\Development\Borsa-Istanbul\borsa-istanbul-backend\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E6CFF0-74D1-43A2-AD12-85788AC8158E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C4DF10-930A-4A89-8998-B994219076B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isyatirim" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="1059">
   <si>
     <t>BRSAN</t>
   </si>
@@ -2015,9 +2015,6 @@
   </si>
   <si>
     <t>Faktoring</t>
-  </si>
-  <si>
-    <t>İçecek</t>
   </si>
   <si>
     <t>EGSER</t>
@@ -3558,8 +3555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C505"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F112" sqref="F112"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C262" sqref="C262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3735,10 +3732,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>969</v>
+      </c>
+      <c r="B16" t="s">
         <v>970</v>
-      </c>
-      <c r="B16" t="s">
-        <v>971</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
@@ -3746,10 +3743,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>971</v>
+      </c>
+      <c r="B17" t="s">
         <v>972</v>
-      </c>
-      <c r="B17" t="s">
-        <v>973</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
@@ -3768,10 +3765,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>973</v>
+      </c>
+      <c r="B19" t="s">
         <v>974</v>
-      </c>
-      <c r="B19" t="s">
-        <v>975</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -3977,13 +3974,13 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
+        <v>773</v>
+      </c>
+      <c r="B38" t="s">
         <v>774</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>775</v>
-      </c>
-      <c r="C38" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -4269,7 +4266,7 @@
         <v>482</v>
       </c>
       <c r="C64" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -4280,7 +4277,7 @@
         <v>484</v>
       </c>
       <c r="C65" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -4291,7 +4288,7 @@
         <v>486</v>
       </c>
       <c r="C66" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -4302,7 +4299,7 @@
         <v>488</v>
       </c>
       <c r="C67" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -4313,7 +4310,7 @@
         <v>490</v>
       </c>
       <c r="C68" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -4324,7 +4321,7 @@
         <v>492</v>
       </c>
       <c r="C69" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -4335,7 +4332,7 @@
         <v>494</v>
       </c>
       <c r="C70" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -4346,7 +4343,7 @@
         <v>496</v>
       </c>
       <c r="C71" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -4357,7 +4354,7 @@
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -4368,7 +4365,7 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -4379,7 +4376,7 @@
         <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -4390,7 +4387,7 @@
         <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -4401,7 +4398,7 @@
         <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -4412,7 +4409,7 @@
         <v>11</v>
       </c>
       <c r="C77" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -4423,7 +4420,7 @@
         <v>13</v>
       </c>
       <c r="C78" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -4434,7 +4431,7 @@
         <v>15</v>
       </c>
       <c r="C79" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -4445,7 +4442,7 @@
         <v>17</v>
       </c>
       <c r="C80" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -4456,7 +4453,7 @@
         <v>19</v>
       </c>
       <c r="C81" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -4467,7 +4464,7 @@
         <v>21</v>
       </c>
       <c r="C82" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -4478,7 +4475,7 @@
         <v>23</v>
       </c>
       <c r="C83" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -4527,57 +4524,57 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
+        <v>977</v>
+      </c>
+      <c r="B88" t="s">
         <v>978</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>979</v>
-      </c>
-      <c r="C88" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
+        <v>980</v>
+      </c>
+      <c r="B89" t="s">
         <v>981</v>
       </c>
-      <c r="B89" t="s">
-        <v>982</v>
-      </c>
       <c r="C89" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
+        <v>982</v>
+      </c>
+      <c r="B90" t="s">
         <v>983</v>
       </c>
-      <c r="B90" t="s">
-        <v>984</v>
-      </c>
       <c r="C90" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
+        <v>984</v>
+      </c>
+      <c r="B91" t="s">
         <v>985</v>
       </c>
-      <c r="B91" t="s">
-        <v>986</v>
-      </c>
       <c r="C91" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
+        <v>987</v>
+      </c>
+      <c r="B92" t="s">
         <v>988</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>989</v>
-      </c>
-      <c r="C92" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -4604,10 +4601,10 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
+        <v>904</v>
+      </c>
+      <c r="B95" t="s">
         <v>905</v>
-      </c>
-      <c r="B95" t="s">
-        <v>906</v>
       </c>
       <c r="C95" t="s">
         <v>102</v>
@@ -4736,10 +4733,10 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
+        <v>906</v>
+      </c>
+      <c r="B107" t="s">
         <v>907</v>
-      </c>
-      <c r="B107" t="s">
-        <v>908</v>
       </c>
       <c r="C107" t="s">
         <v>102</v>
@@ -4978,10 +4975,10 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
+        <v>954</v>
+      </c>
+      <c r="B129" t="s">
         <v>955</v>
-      </c>
-      <c r="B129" t="s">
-        <v>956</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>102</v>
@@ -4995,18 +4992,18 @@
         <v>507</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
+        <v>908</v>
+      </c>
+      <c r="B131" t="s">
         <v>909</v>
       </c>
-      <c r="B131" t="s">
-        <v>910</v>
-      </c>
       <c r="C131" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -5017,18 +5014,18 @@
         <v>509</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
+        <v>910</v>
+      </c>
+      <c r="B133" t="s">
         <v>911</v>
       </c>
-      <c r="B133" t="s">
-        <v>912</v>
-      </c>
       <c r="C133" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -5039,7 +5036,7 @@
         <v>511</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -5050,7 +5047,7 @@
         <v>513</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -5061,7 +5058,7 @@
         <v>515</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -5069,7 +5066,7 @@
         <v>169</v>
       </c>
       <c r="B137" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C137" t="s">
         <v>170</v>
@@ -5077,10 +5074,10 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
+        <v>912</v>
+      </c>
+      <c r="B138" t="s">
         <v>913</v>
-      </c>
-      <c r="B138" t="s">
-        <v>914</v>
       </c>
       <c r="C138" t="s">
         <v>170</v>
@@ -5220,10 +5217,10 @@
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
+        <v>914</v>
+      </c>
+      <c r="B151" t="s">
         <v>915</v>
-      </c>
-      <c r="B151" t="s">
-        <v>916</v>
       </c>
       <c r="C151" t="s">
         <v>177</v>
@@ -5264,10 +5261,10 @@
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
+        <v>916</v>
+      </c>
+      <c r="B155" t="s">
         <v>917</v>
-      </c>
-      <c r="B155" t="s">
-        <v>918</v>
       </c>
       <c r="C155" t="s">
         <v>177</v>
@@ -5319,10 +5316,10 @@
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
+        <v>918</v>
+      </c>
+      <c r="B160" t="s">
         <v>919</v>
-      </c>
-      <c r="B160" t="s">
-        <v>920</v>
       </c>
       <c r="C160" t="s">
         <v>177</v>
@@ -5341,10 +5338,10 @@
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
+        <v>920</v>
+      </c>
+      <c r="B162" t="s">
         <v>921</v>
-      </c>
-      <c r="B162" t="s">
-        <v>922</v>
       </c>
       <c r="C162" t="s">
         <v>177</v>
@@ -6067,24 +6064,24 @@
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
+        <v>922</v>
+      </c>
+      <c r="B228" t="s">
         <v>923</v>
       </c>
-      <c r="B228" t="s">
+      <c r="C228" t="s">
         <v>924</v>
-      </c>
-      <c r="C228" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
+        <v>925</v>
+      </c>
+      <c r="B229" t="s">
         <v>926</v>
       </c>
-      <c r="B229" t="s">
-        <v>927</v>
-      </c>
       <c r="C229" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -6095,7 +6092,7 @@
         <v>235</v>
       </c>
       <c r="C230" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -6106,7 +6103,7 @@
         <v>237</v>
       </c>
       <c r="C231" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -6117,7 +6114,7 @@
         <v>239</v>
       </c>
       <c r="C232" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -6128,7 +6125,7 @@
         <v>241</v>
       </c>
       <c r="C233" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -6139,7 +6136,7 @@
         <v>243</v>
       </c>
       <c r="C234" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -6150,7 +6147,7 @@
         <v>245</v>
       </c>
       <c r="C235" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -6161,7 +6158,7 @@
         <v>247</v>
       </c>
       <c r="C236" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -6172,7 +6169,7 @@
         <v>249</v>
       </c>
       <c r="C237" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -6183,7 +6180,7 @@
         <v>251</v>
       </c>
       <c r="C238" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -6194,7 +6191,7 @@
         <v>253</v>
       </c>
       <c r="C239" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -6205,7 +6202,7 @@
         <v>255</v>
       </c>
       <c r="C240" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -6216,7 +6213,7 @@
         <v>257</v>
       </c>
       <c r="C241" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -6227,7 +6224,7 @@
         <v>259</v>
       </c>
       <c r="C242" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -6238,7 +6235,7 @@
         <v>261</v>
       </c>
       <c r="C243" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -6249,7 +6246,7 @@
         <v>263</v>
       </c>
       <c r="C244" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -6260,7 +6257,7 @@
         <v>265</v>
       </c>
       <c r="C245" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -6271,7 +6268,7 @@
         <v>267</v>
       </c>
       <c r="C246" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -6282,7 +6279,7 @@
         <v>269</v>
       </c>
       <c r="C247" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -6293,7 +6290,7 @@
         <v>271</v>
       </c>
       <c r="C248" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -6304,7 +6301,7 @@
         <v>273</v>
       </c>
       <c r="C249" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -6315,7 +6312,7 @@
         <v>275</v>
       </c>
       <c r="C250" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -6326,7 +6323,7 @@
         <v>277</v>
       </c>
       <c r="C251" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -6337,7 +6334,7 @@
         <v>279</v>
       </c>
       <c r="C252" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -6348,7 +6345,7 @@
         <v>281</v>
       </c>
       <c r="C253" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -6359,7 +6356,7 @@
         <v>283</v>
       </c>
       <c r="C254" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -6370,7 +6367,7 @@
         <v>285</v>
       </c>
       <c r="C255" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -6381,7 +6378,7 @@
         <v>287</v>
       </c>
       <c r="C256" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -6392,7 +6389,7 @@
         <v>289</v>
       </c>
       <c r="C257" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -6403,7 +6400,7 @@
         <v>291</v>
       </c>
       <c r="C258" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -6414,7 +6411,7 @@
         <v>293</v>
       </c>
       <c r="C259" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -6425,7 +6422,7 @@
         <v>295</v>
       </c>
       <c r="C260" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="261" spans="1:3">
@@ -6436,103 +6433,103 @@
         <v>297</v>
       </c>
       <c r="C261" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
-        <v>298</v>
+        <v>776</v>
       </c>
       <c r="B262" t="s">
-        <v>299</v>
-      </c>
-      <c r="C262" s="1" t="s">
-        <v>665</v>
+        <v>777</v>
+      </c>
+      <c r="C262" t="s">
+        <v>778</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="B263" t="s">
+        <v>780</v>
+      </c>
+      <c r="C263" t="s">
         <v>778</v>
-      </c>
-      <c r="C263" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B264" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C264" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B265" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C265" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" t="s">
-        <v>784</v>
+        <v>897</v>
       </c>
       <c r="B266" t="s">
-        <v>785</v>
+        <v>898</v>
       </c>
       <c r="C266" t="s">
-        <v>779</v>
+        <v>899</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="B267" t="s">
+        <v>901</v>
+      </c>
+      <c r="C267" t="s">
         <v>899</v>
-      </c>
-      <c r="C267" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B268" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C268" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" t="s">
-        <v>903</v>
+        <v>927</v>
       </c>
       <c r="B269" t="s">
-        <v>904</v>
-      </c>
-      <c r="C269" t="s">
-        <v>900</v>
+        <v>928</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="270" spans="1:3">
       <c r="A270" t="s">
-        <v>928</v>
+        <v>316</v>
       </c>
       <c r="B270" t="s">
-        <v>929</v>
+        <v>317</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>318</v>
@@ -6540,10 +6537,10 @@
     </row>
     <row r="271" spans="1:3">
       <c r="A271" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B271" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>318</v>
@@ -6551,10 +6548,10 @@
     </row>
     <row r="272" spans="1:3">
       <c r="A272" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B272" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>318</v>
@@ -6562,10 +6559,10 @@
     </row>
     <row r="273" spans="1:3">
       <c r="A273" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B273" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>318</v>
@@ -6573,10 +6570,10 @@
     </row>
     <row r="274" spans="1:3">
       <c r="A274" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B274" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>318</v>
@@ -6584,373 +6581,373 @@
     </row>
     <row r="275" spans="1:3">
       <c r="A275" t="s">
-        <v>325</v>
+        <v>785</v>
       </c>
       <c r="B275" t="s">
-        <v>326</v>
-      </c>
-      <c r="C275" s="1" t="s">
-        <v>318</v>
+        <v>786</v>
+      </c>
+      <c r="C275" t="s">
+        <v>787</v>
       </c>
     </row>
     <row r="276" spans="1:3">
       <c r="A276" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="B276" t="s">
+        <v>789</v>
+      </c>
+      <c r="C276" t="s">
         <v>787</v>
-      </c>
-      <c r="C276" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="277" spans="1:3">
       <c r="A277" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B277" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C277" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="278" spans="1:3">
       <c r="A278" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B278" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C278" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B279" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C279" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="280" spans="1:3">
       <c r="A280" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B280" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C280" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="281" spans="1:3">
       <c r="A281" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B281" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="C281" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="282" spans="1:3">
       <c r="A282" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B282" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C282" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B283" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C283" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="284" spans="1:3">
       <c r="A284" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B284" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C284" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="285" spans="1:3">
       <c r="A285" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B285" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C285" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="286" spans="1:3">
       <c r="A286" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B286" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="C286" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="287" spans="1:3">
       <c r="A287" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B287" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C287" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="288" spans="1:3">
       <c r="A288" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B288" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="C288" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="289" spans="1:3">
       <c r="A289" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B289" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C289" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="290" spans="1:3">
       <c r="A290" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="B290" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C290" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="291" spans="1:3">
       <c r="A291" t="s">
-        <v>817</v>
+        <v>929</v>
       </c>
       <c r="B291" t="s">
-        <v>818</v>
+        <v>930</v>
       </c>
       <c r="C291" t="s">
-        <v>788</v>
+        <v>931</v>
       </c>
     </row>
     <row r="292" spans="1:3">
       <c r="A292" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="B292" t="s">
+        <v>933</v>
+      </c>
+      <c r="C292" t="s">
         <v>931</v>
-      </c>
-      <c r="C292" t="s">
-        <v>932</v>
       </c>
     </row>
     <row r="293" spans="1:3">
       <c r="A293" t="s">
-        <v>933</v>
+        <v>733</v>
       </c>
       <c r="B293" t="s">
-        <v>934</v>
+        <v>734</v>
       </c>
       <c r="C293" t="s">
-        <v>932</v>
+        <v>735</v>
       </c>
     </row>
     <row r="294" spans="1:3">
       <c r="A294" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B294" t="s">
+        <v>737</v>
+      </c>
+      <c r="C294" t="s">
         <v>735</v>
-      </c>
-      <c r="C294" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="295" spans="1:3">
       <c r="A295" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B295" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="C295" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="296" spans="1:3">
       <c r="A296" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B296" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C296" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="297" spans="1:3">
       <c r="A297" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B297" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C297" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="298" spans="1:3">
       <c r="A298" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B298" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C298" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="299" spans="1:3">
       <c r="A299" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B299" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C299" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="300" spans="1:3">
       <c r="A300" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B300" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C300" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="301" spans="1:3">
       <c r="A301" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B301" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="C301" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="302" spans="1:3">
       <c r="A302" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B302" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="C302" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="303" spans="1:3">
       <c r="A303" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B303" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C303" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="304" spans="1:3">
       <c r="A304" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B304" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C304" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="305" spans="1:3">
       <c r="A305" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B305" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C305" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="306" spans="1:3">
       <c r="A306" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B306" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C306" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="307" spans="1:3">
       <c r="A307" t="s">
-        <v>761</v>
+        <v>327</v>
       </c>
       <c r="B307" t="s">
-        <v>762</v>
+        <v>328</v>
       </c>
       <c r="C307" t="s">
-        <v>736</v>
+        <v>329</v>
       </c>
     </row>
     <row r="308" spans="1:3">
       <c r="A308" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B308" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="C308" t="s">
         <v>329</v>
@@ -6958,10 +6955,10 @@
     </row>
     <row r="309" spans="1:3">
       <c r="A309" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B309" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C309" t="s">
         <v>329</v>
@@ -6969,10 +6966,10 @@
     </row>
     <row r="310" spans="1:3">
       <c r="A310" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B310" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C310" t="s">
         <v>329</v>
@@ -6980,10 +6977,10 @@
     </row>
     <row r="311" spans="1:3">
       <c r="A311" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B311" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C311" t="s">
         <v>329</v>
@@ -6991,10 +6988,10 @@
     </row>
     <row r="312" spans="1:3">
       <c r="A312" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B312" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C312" t="s">
         <v>329</v>
@@ -7002,10 +6999,10 @@
     </row>
     <row r="313" spans="1:3">
       <c r="A313" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B313" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C313" t="s">
         <v>329</v>
@@ -7013,10 +7010,10 @@
     </row>
     <row r="314" spans="1:3">
       <c r="A314" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B314" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C314" t="s">
         <v>329</v>
@@ -7024,10 +7021,10 @@
     </row>
     <row r="315" spans="1:3">
       <c r="A315" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B315" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C315" t="s">
         <v>329</v>
@@ -7035,10 +7032,10 @@
     </row>
     <row r="316" spans="1:3">
       <c r="A316" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B316" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C316" t="s">
         <v>329</v>
@@ -7046,10 +7043,10 @@
     </row>
     <row r="317" spans="1:3">
       <c r="A317" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B317" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C317" t="s">
         <v>329</v>
@@ -7057,10 +7054,10 @@
     </row>
     <row r="318" spans="1:3">
       <c r="A318" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B318" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C318" t="s">
         <v>329</v>
@@ -7068,10 +7065,10 @@
     </row>
     <row r="319" spans="1:3">
       <c r="A319" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B319" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C319" t="s">
         <v>329</v>
@@ -7079,10 +7076,10 @@
     </row>
     <row r="320" spans="1:3">
       <c r="A320" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B320" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C320" t="s">
         <v>329</v>
@@ -7090,10 +7087,10 @@
     </row>
     <row r="321" spans="1:3">
       <c r="A321" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B321" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C321" t="s">
         <v>329</v>
@@ -7101,10 +7098,10 @@
     </row>
     <row r="322" spans="1:3">
       <c r="A322" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B322" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C322" t="s">
         <v>329</v>
@@ -7112,178 +7109,178 @@
     </row>
     <row r="323" spans="1:3">
       <c r="A323" t="s">
-        <v>358</v>
+        <v>934</v>
       </c>
       <c r="B323" t="s">
-        <v>359</v>
+        <v>935</v>
       </c>
       <c r="C323" t="s">
-        <v>329</v>
+        <v>936</v>
       </c>
     </row>
     <row r="324" spans="1:3">
       <c r="A324" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="B324" t="s">
+        <v>938</v>
+      </c>
+      <c r="C324" t="s">
         <v>936</v>
-      </c>
-      <c r="C324" t="s">
-        <v>937</v>
       </c>
     </row>
     <row r="325" spans="1:3">
       <c r="A325" t="s">
-        <v>938</v>
+        <v>762</v>
       </c>
       <c r="B325" t="s">
-        <v>939</v>
+        <v>763</v>
       </c>
       <c r="C325" t="s">
-        <v>937</v>
+        <v>764</v>
       </c>
     </row>
     <row r="326" spans="1:3">
       <c r="A326" t="s">
-        <v>763</v>
+        <v>991</v>
       </c>
       <c r="B326" t="s">
+        <v>992</v>
+      </c>
+      <c r="C326" t="s">
         <v>764</v>
-      </c>
-      <c r="C326" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="327" spans="1:3">
       <c r="A327" t="s">
-        <v>992</v>
+        <v>765</v>
       </c>
       <c r="B327" t="s">
-        <v>993</v>
+        <v>766</v>
       </c>
       <c r="C327" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="328" spans="1:3">
       <c r="A328" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B328" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="C328" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="329" spans="1:3">
       <c r="A329" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B329" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C329" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="330" spans="1:3">
       <c r="A330" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="B330" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C330" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="331" spans="1:3">
       <c r="A331" t="s">
-        <v>772</v>
+        <v>939</v>
       </c>
       <c r="B331" t="s">
-        <v>773</v>
+        <v>940</v>
       </c>
       <c r="C331" t="s">
-        <v>765</v>
+        <v>941</v>
       </c>
     </row>
     <row r="332" spans="1:3">
       <c r="A332" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="B332" t="s">
+        <v>943</v>
+      </c>
+      <c r="C332" t="s">
         <v>941</v>
-      </c>
-      <c r="C332" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="333" spans="1:3">
       <c r="A333" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B333" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C333" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="334" spans="1:3">
       <c r="A334" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B334" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="C334" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="335" spans="1:3">
       <c r="A335" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B335" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="C335" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="336" spans="1:3">
       <c r="A336" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B336" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C336" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="337" spans="1:3">
       <c r="A337" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B337" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="C337" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="338" spans="1:3">
       <c r="A338" t="s">
-        <v>953</v>
+        <v>298</v>
       </c>
       <c r="B338" t="s">
-        <v>954</v>
+        <v>299</v>
       </c>
       <c r="C338" t="s">
-        <v>942</v>
+        <v>993</v>
       </c>
     </row>
     <row r="339" spans="1:3">
@@ -7294,7 +7291,7 @@
         <v>301</v>
       </c>
       <c r="C339" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="340" spans="1:3">
@@ -7305,7 +7302,7 @@
         <v>303</v>
       </c>
       <c r="C340" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="341" spans="1:3">
@@ -7316,7 +7313,7 @@
         <v>305</v>
       </c>
       <c r="C341" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="342" spans="1:3">
@@ -7327,7 +7324,7 @@
         <v>307</v>
       </c>
       <c r="C342" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="343" spans="1:3">
@@ -7338,7 +7335,7 @@
         <v>309</v>
       </c>
       <c r="C343" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="344" spans="1:3">
@@ -7349,7 +7346,7 @@
         <v>311</v>
       </c>
       <c r="C344" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="345" spans="1:3">
@@ -7360,7 +7357,7 @@
         <v>313</v>
       </c>
       <c r="C345" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="346" spans="1:3">
@@ -7371,73 +7368,73 @@
         <v>315</v>
       </c>
       <c r="C346" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="347" spans="1:3">
       <c r="A347" t="s">
+        <v>956</v>
+      </c>
+      <c r="B347" t="s">
         <v>957</v>
       </c>
-      <c r="B347" t="s">
+      <c r="C347" t="s">
         <v>958</v>
-      </c>
-      <c r="C347" t="s">
-        <v>959</v>
       </c>
     </row>
     <row r="348" spans="1:3">
       <c r="A348" t="s">
+        <v>959</v>
+      </c>
+      <c r="B348" t="s">
         <v>960</v>
       </c>
-      <c r="B348" t="s">
-        <v>961</v>
-      </c>
       <c r="C348" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="349" spans="1:3">
       <c r="A349" t="s">
+        <v>961</v>
+      </c>
+      <c r="B349" t="s">
         <v>962</v>
       </c>
-      <c r="B349" t="s">
-        <v>963</v>
-      </c>
       <c r="C349" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="350" spans="1:3">
       <c r="A350" t="s">
+        <v>963</v>
+      </c>
+      <c r="B350" t="s">
         <v>964</v>
       </c>
-      <c r="B350" t="s">
-        <v>965</v>
-      </c>
       <c r="C350" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="351" spans="1:3">
       <c r="A351" t="s">
+        <v>965</v>
+      </c>
+      <c r="B351" t="s">
         <v>966</v>
       </c>
-      <c r="B351" t="s">
-        <v>967</v>
-      </c>
       <c r="C351" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="352" spans="1:3">
       <c r="A352" t="s">
+        <v>967</v>
+      </c>
+      <c r="B352" t="s">
         <v>968</v>
       </c>
-      <c r="B352" t="s">
-        <v>969</v>
-      </c>
       <c r="C352" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="353" spans="1:3">
@@ -7530,167 +7527,167 @@
     </row>
     <row r="361" spans="1:3">
       <c r="A361" t="s">
+        <v>994</v>
+      </c>
+      <c r="B361" t="s">
         <v>995</v>
       </c>
-      <c r="B361" t="s">
+      <c r="C361" t="s">
         <v>996</v>
-      </c>
-      <c r="C361" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="362" spans="1:3">
       <c r="A362" t="s">
+        <v>997</v>
+      </c>
+      <c r="B362" t="s">
         <v>998</v>
       </c>
-      <c r="B362" t="s">
-        <v>999</v>
-      </c>
       <c r="C362" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="363" spans="1:3">
       <c r="A363" t="s">
+        <v>818</v>
+      </c>
+      <c r="B363" t="s">
         <v>819</v>
       </c>
-      <c r="B363" t="s">
+      <c r="C363" t="s">
         <v>820</v>
-      </c>
-      <c r="C363" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="364" spans="1:3">
       <c r="A364" t="s">
+        <v>821</v>
+      </c>
+      <c r="B364" t="s">
         <v>822</v>
       </c>
-      <c r="B364" t="s">
-        <v>823</v>
-      </c>
       <c r="C364" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="365" spans="1:3">
       <c r="A365" t="s">
+        <v>823</v>
+      </c>
+      <c r="B365" t="s">
         <v>824</v>
       </c>
-      <c r="B365" t="s">
-        <v>825</v>
-      </c>
       <c r="C365" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="366" spans="1:3">
       <c r="A366" t="s">
+        <v>825</v>
+      </c>
+      <c r="B366" t="s">
         <v>826</v>
       </c>
-      <c r="B366" t="s">
-        <v>827</v>
-      </c>
       <c r="C366" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="367" spans="1:3">
       <c r="A367" t="s">
+        <v>827</v>
+      </c>
+      <c r="B367" t="s">
         <v>828</v>
       </c>
-      <c r="B367" t="s">
-        <v>829</v>
-      </c>
       <c r="C367" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="368" spans="1:3">
       <c r="A368" t="s">
+        <v>829</v>
+      </c>
+      <c r="B368" t="s">
         <v>830</v>
       </c>
-      <c r="B368" t="s">
-        <v>831</v>
-      </c>
       <c r="C368" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="369" spans="1:3">
       <c r="A369" t="s">
+        <v>831</v>
+      </c>
+      <c r="B369" t="s">
         <v>832</v>
       </c>
-      <c r="B369" t="s">
-        <v>833</v>
-      </c>
       <c r="C369" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="370" spans="1:3">
       <c r="A370" t="s">
+        <v>833</v>
+      </c>
+      <c r="B370" t="s">
         <v>834</v>
       </c>
-      <c r="B370" t="s">
-        <v>835</v>
-      </c>
       <c r="C370" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="371" spans="1:3">
       <c r="A371" t="s">
+        <v>835</v>
+      </c>
+      <c r="B371" t="s">
         <v>836</v>
       </c>
-      <c r="B371" t="s">
-        <v>837</v>
-      </c>
       <c r="C371" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="372" spans="1:3">
       <c r="A372" t="s">
+        <v>837</v>
+      </c>
+      <c r="B372" t="s">
         <v>838</v>
       </c>
-      <c r="B372" t="s">
-        <v>839</v>
-      </c>
       <c r="C372" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="373" spans="1:3">
       <c r="A373" t="s">
+        <v>999</v>
+      </c>
+      <c r="B373" t="s">
         <v>1000</v>
       </c>
-      <c r="B373" t="s">
+      <c r="C373" t="s">
         <v>1001</v>
-      </c>
-      <c r="C373" t="s">
-        <v>1002</v>
       </c>
     </row>
     <row r="374" spans="1:3">
       <c r="A374" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B374" t="s">
         <v>1003</v>
       </c>
-      <c r="B374" t="s">
-        <v>1004</v>
-      </c>
       <c r="C374" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="375" spans="1:3">
       <c r="A375" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B375" t="s">
         <v>1005</v>
       </c>
-      <c r="B375" t="s">
-        <v>1006</v>
-      </c>
       <c r="C375" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="376" spans="1:3">
@@ -7701,7 +7698,7 @@
         <v>378</v>
       </c>
       <c r="C376" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="377" spans="1:3">
@@ -7712,7 +7709,7 @@
         <v>380</v>
       </c>
       <c r="C377" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="378" spans="1:3">
@@ -7723,7 +7720,7 @@
         <v>382</v>
       </c>
       <c r="C378" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="379" spans="1:3">
@@ -7734,7 +7731,7 @@
         <v>384</v>
       </c>
       <c r="C379" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="380" spans="1:3">
@@ -7745,7 +7742,7 @@
         <v>386</v>
       </c>
       <c r="C380" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="381" spans="1:3">
@@ -7756,18 +7753,18 @@
         <v>388</v>
       </c>
       <c r="C381" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="382" spans="1:3">
       <c r="A382" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B382" t="s">
         <v>1008</v>
       </c>
-      <c r="B382" t="s">
-        <v>1009</v>
-      </c>
       <c r="C382" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="383" spans="1:3">
@@ -7778,7 +7775,7 @@
         <v>390</v>
       </c>
       <c r="C383" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="384" spans="1:3">
@@ -7789,7 +7786,7 @@
         <v>392</v>
       </c>
       <c r="C384" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="385" spans="1:3">
@@ -7800,7 +7797,7 @@
         <v>394</v>
       </c>
       <c r="C385" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="386" spans="1:3">
@@ -7811,7 +7808,7 @@
         <v>396</v>
       </c>
       <c r="C386" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="387" spans="1:3">
@@ -7822,7 +7819,7 @@
         <v>398</v>
       </c>
       <c r="C387" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="388" spans="1:3">
@@ -7833,7 +7830,7 @@
         <v>400</v>
       </c>
       <c r="C388" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="389" spans="1:3">
@@ -7904,200 +7901,200 @@
     </row>
     <row r="395" spans="1:3">
       <c r="A395" t="s">
+        <v>839</v>
+      </c>
+      <c r="B395" t="s">
         <v>840</v>
       </c>
-      <c r="B395" t="s">
+      <c r="C395" t="s">
         <v>841</v>
-      </c>
-      <c r="C395" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="396" spans="1:3">
       <c r="A396" t="s">
+        <v>842</v>
+      </c>
+      <c r="B396" t="s">
         <v>843</v>
       </c>
-      <c r="B396" t="s">
-        <v>844</v>
-      </c>
       <c r="C396" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="397" spans="1:3">
       <c r="A397" t="s">
+        <v>844</v>
+      </c>
+      <c r="B397" t="s">
         <v>845</v>
       </c>
-      <c r="B397" t="s">
-        <v>846</v>
-      </c>
       <c r="C397" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="398" spans="1:3">
       <c r="A398" t="s">
+        <v>846</v>
+      </c>
+      <c r="B398" t="s">
         <v>847</v>
       </c>
-      <c r="B398" t="s">
-        <v>848</v>
-      </c>
       <c r="C398" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="399" spans="1:3">
       <c r="A399" t="s">
+        <v>848</v>
+      </c>
+      <c r="B399" t="s">
         <v>849</v>
       </c>
-      <c r="B399" t="s">
-        <v>850</v>
-      </c>
       <c r="C399" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="400" spans="1:3">
       <c r="A400" t="s">
+        <v>850</v>
+      </c>
+      <c r="B400" t="s">
         <v>851</v>
       </c>
-      <c r="B400" t="s">
-        <v>852</v>
-      </c>
       <c r="C400" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="401" spans="1:3">
       <c r="A401" t="s">
+        <v>852</v>
+      </c>
+      <c r="B401" t="s">
         <v>853</v>
       </c>
-      <c r="B401" t="s">
-        <v>854</v>
-      </c>
       <c r="C401" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="402" spans="1:3">
       <c r="A402" t="s">
+        <v>854</v>
+      </c>
+      <c r="B402" t="s">
         <v>855</v>
       </c>
-      <c r="B402" t="s">
-        <v>856</v>
-      </c>
       <c r="C402" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="403" spans="1:3">
       <c r="A403" t="s">
+        <v>856</v>
+      </c>
+      <c r="B403" t="s">
         <v>857</v>
       </c>
-      <c r="B403" t="s">
-        <v>858</v>
-      </c>
       <c r="C403" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="404" spans="1:3">
       <c r="A404" t="s">
+        <v>858</v>
+      </c>
+      <c r="B404" t="s">
         <v>859</v>
       </c>
-      <c r="B404" t="s">
-        <v>860</v>
-      </c>
       <c r="C404" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="405" spans="1:3">
       <c r="A405" t="s">
+        <v>860</v>
+      </c>
+      <c r="B405" t="s">
         <v>861</v>
       </c>
-      <c r="B405" t="s">
-        <v>862</v>
-      </c>
       <c r="C405" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="406" spans="1:3">
       <c r="A406" t="s">
+        <v>862</v>
+      </c>
+      <c r="B406" t="s">
         <v>863</v>
       </c>
-      <c r="B406" t="s">
-        <v>864</v>
-      </c>
       <c r="C406" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="407" spans="1:3">
       <c r="A407" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B407" t="s">
         <v>1010</v>
       </c>
-      <c r="B407" t="s">
+      <c r="C407" t="s">
         <v>1011</v>
-      </c>
-      <c r="C407" t="s">
-        <v>1012</v>
       </c>
     </row>
     <row r="408" spans="1:3">
       <c r="A408" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B408" t="s">
         <v>1013</v>
       </c>
-      <c r="B408" t="s">
-        <v>1014</v>
-      </c>
       <c r="C408" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="409" spans="1:3">
       <c r="A409" t="s">
+        <v>665</v>
+      </c>
+      <c r="B409" t="s">
         <v>666</v>
       </c>
-      <c r="B409" t="s">
+      <c r="C409" t="s">
         <v>667</v>
-      </c>
-      <c r="C409" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="410" spans="1:3">
       <c r="A410" t="s">
+        <v>668</v>
+      </c>
+      <c r="B410" t="s">
         <v>669</v>
       </c>
-      <c r="B410" t="s">
-        <v>670</v>
-      </c>
       <c r="C410" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="411" spans="1:3">
       <c r="A411" t="s">
+        <v>670</v>
+      </c>
+      <c r="B411" t="s">
         <v>671</v>
       </c>
-      <c r="B411" t="s">
-        <v>672</v>
-      </c>
       <c r="C411" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="412" spans="1:3">
       <c r="A412" t="s">
+        <v>672</v>
+      </c>
+      <c r="B412" t="s">
         <v>673</v>
       </c>
-      <c r="B412" t="s">
-        <v>674</v>
-      </c>
       <c r="C412" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="413" spans="1:3">
@@ -8168,90 +8165,90 @@
     </row>
     <row r="419" spans="1:3">
       <c r="A419" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B419" t="s">
         <v>1015</v>
       </c>
-      <c r="B419" t="s">
+      <c r="C419" t="s">
         <v>1016</v>
-      </c>
-      <c r="C419" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="420" spans="1:3">
       <c r="A420" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B420" t="s">
         <v>1018</v>
       </c>
-      <c r="B420" t="s">
-        <v>1019</v>
-      </c>
       <c r="C420" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="421" spans="1:3">
       <c r="A421" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B421" t="s">
         <v>1020</v>
       </c>
-      <c r="B421" t="s">
-        <v>1021</v>
-      </c>
       <c r="C421" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="422" spans="1:3">
       <c r="A422" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B422" t="s">
         <v>1022</v>
       </c>
-      <c r="B422" t="s">
-        <v>1023</v>
-      </c>
       <c r="C422" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="423" spans="1:3">
       <c r="A423" t="s">
+        <v>674</v>
+      </c>
+      <c r="B423" t="s">
         <v>675</v>
       </c>
-      <c r="B423" t="s">
+      <c r="C423" t="s">
         <v>676</v>
-      </c>
-      <c r="C423" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="424" spans="1:3">
       <c r="A424" t="s">
+        <v>677</v>
+      </c>
+      <c r="B424" t="s">
         <v>678</v>
       </c>
-      <c r="B424" t="s">
-        <v>679</v>
-      </c>
       <c r="C424" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="425" spans="1:3">
       <c r="A425" t="s">
+        <v>679</v>
+      </c>
+      <c r="B425" t="s">
         <v>680</v>
       </c>
-      <c r="B425" t="s">
-        <v>681</v>
-      </c>
       <c r="C425" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="426" spans="1:3">
       <c r="A426" t="s">
+        <v>681</v>
+      </c>
+      <c r="B426" t="s">
         <v>682</v>
       </c>
-      <c r="B426" t="s">
-        <v>683</v>
-      </c>
       <c r="C426" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="427" spans="1:3">
@@ -8432,453 +8429,453 @@
     </row>
     <row r="443" spans="1:3">
       <c r="A443" t="s">
+        <v>683</v>
+      </c>
+      <c r="B443" t="s">
         <v>684</v>
       </c>
-      <c r="B443" t="s">
-        <v>685</v>
-      </c>
       <c r="C443" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="444" spans="1:3">
       <c r="A444" t="s">
+        <v>685</v>
+      </c>
+      <c r="B444" t="s">
         <v>686</v>
       </c>
-      <c r="B444" t="s">
-        <v>687</v>
-      </c>
       <c r="C444" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="445" spans="1:3">
       <c r="A445" t="s">
+        <v>687</v>
+      </c>
+      <c r="B445" t="s">
         <v>688</v>
       </c>
-      <c r="B445" t="s">
-        <v>689</v>
-      </c>
       <c r="C445" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="446" spans="1:3">
       <c r="A446" t="s">
+        <v>689</v>
+      </c>
+      <c r="B446" t="s">
         <v>690</v>
       </c>
-      <c r="B446" t="s">
-        <v>691</v>
-      </c>
       <c r="C446" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="447" spans="1:3">
       <c r="A447" t="s">
+        <v>691</v>
+      </c>
+      <c r="B447" t="s">
         <v>692</v>
       </c>
-      <c r="B447" t="s">
-        <v>693</v>
-      </c>
       <c r="C447" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="448" spans="1:3">
       <c r="A448" t="s">
+        <v>693</v>
+      </c>
+      <c r="B448" t="s">
         <v>694</v>
       </c>
-      <c r="B448" t="s">
-        <v>695</v>
-      </c>
       <c r="C448" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="449" spans="1:3">
       <c r="A449" t="s">
+        <v>695</v>
+      </c>
+      <c r="B449" t="s">
         <v>696</v>
       </c>
-      <c r="B449" t="s">
-        <v>697</v>
-      </c>
       <c r="C449" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="450" spans="1:3">
       <c r="A450" t="s">
+        <v>697</v>
+      </c>
+      <c r="B450" t="s">
         <v>698</v>
       </c>
-      <c r="B450" t="s">
-        <v>699</v>
-      </c>
       <c r="C450" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="451" spans="1:3">
       <c r="A451" t="s">
+        <v>699</v>
+      </c>
+      <c r="B451" t="s">
         <v>700</v>
       </c>
-      <c r="B451" t="s">
-        <v>701</v>
-      </c>
       <c r="C451" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="452" spans="1:3">
       <c r="A452" t="s">
+        <v>701</v>
+      </c>
+      <c r="B452" t="s">
         <v>702</v>
       </c>
-      <c r="B452" t="s">
-        <v>703</v>
-      </c>
       <c r="C452" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="453" spans="1:3">
       <c r="A453" t="s">
+        <v>703</v>
+      </c>
+      <c r="B453" t="s">
         <v>704</v>
       </c>
-      <c r="B453" t="s">
-        <v>705</v>
-      </c>
       <c r="C453" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="454" spans="1:3">
       <c r="A454" t="s">
+        <v>705</v>
+      </c>
+      <c r="B454" t="s">
         <v>706</v>
       </c>
-      <c r="B454" t="s">
-        <v>707</v>
-      </c>
       <c r="C454" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="455" spans="1:3">
       <c r="A455" t="s">
+        <v>707</v>
+      </c>
+      <c r="B455" t="s">
         <v>708</v>
       </c>
-      <c r="B455" t="s">
-        <v>709</v>
-      </c>
       <c r="C455" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="456" spans="1:3">
       <c r="A456" t="s">
+        <v>709</v>
+      </c>
+      <c r="B456" t="s">
         <v>710</v>
       </c>
-      <c r="B456" t="s">
-        <v>711</v>
-      </c>
       <c r="C456" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="457" spans="1:3">
       <c r="A457" t="s">
+        <v>711</v>
+      </c>
+      <c r="B457" t="s">
         <v>712</v>
       </c>
-      <c r="B457" t="s">
-        <v>713</v>
-      </c>
       <c r="C457" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="458" spans="1:3">
       <c r="A458" t="s">
+        <v>713</v>
+      </c>
+      <c r="B458" t="s">
         <v>714</v>
       </c>
-      <c r="B458" t="s">
-        <v>715</v>
-      </c>
       <c r="C458" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="459" spans="1:3">
       <c r="A459" t="s">
+        <v>715</v>
+      </c>
+      <c r="B459" t="s">
         <v>716</v>
       </c>
-      <c r="B459" t="s">
-        <v>717</v>
-      </c>
       <c r="C459" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="460" spans="1:3">
       <c r="A460" t="s">
+        <v>717</v>
+      </c>
+      <c r="B460" t="s">
         <v>718</v>
       </c>
-      <c r="B460" t="s">
-        <v>719</v>
-      </c>
       <c r="C460" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="461" spans="1:3">
       <c r="A461" t="s">
+        <v>719</v>
+      </c>
+      <c r="B461" t="s">
         <v>720</v>
       </c>
-      <c r="B461" t="s">
-        <v>721</v>
-      </c>
       <c r="C461" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="462" spans="1:3">
       <c r="A462" t="s">
+        <v>721</v>
+      </c>
+      <c r="B462" t="s">
         <v>722</v>
       </c>
-      <c r="B462" t="s">
-        <v>723</v>
-      </c>
       <c r="C462" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="463" spans="1:3">
       <c r="A463" t="s">
+        <v>723</v>
+      </c>
+      <c r="B463" t="s">
         <v>724</v>
       </c>
-      <c r="B463" t="s">
-        <v>725</v>
-      </c>
       <c r="C463" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="464" spans="1:3">
       <c r="A464" t="s">
+        <v>725</v>
+      </c>
+      <c r="B464" t="s">
         <v>726</v>
       </c>
-      <c r="B464" t="s">
-        <v>727</v>
-      </c>
       <c r="C464" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="465" spans="1:3">
       <c r="A465" t="s">
+        <v>727</v>
+      </c>
+      <c r="B465" t="s">
         <v>728</v>
       </c>
-      <c r="B465" t="s">
-        <v>729</v>
-      </c>
       <c r="C465" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="466" spans="1:3">
       <c r="A466" t="s">
+        <v>729</v>
+      </c>
+      <c r="B466" t="s">
         <v>730</v>
       </c>
-      <c r="B466" t="s">
-        <v>731</v>
-      </c>
       <c r="C466" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="467" spans="1:3">
       <c r="A467" t="s">
+        <v>731</v>
+      </c>
+      <c r="B467" t="s">
         <v>732</v>
       </c>
-      <c r="B467" t="s">
-        <v>733</v>
-      </c>
       <c r="C467" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="468" spans="1:3">
       <c r="A468" t="s">
+        <v>864</v>
+      </c>
+      <c r="B468" t="s">
         <v>865</v>
       </c>
-      <c r="B468" t="s">
+      <c r="C468" t="s">
         <v>866</v>
-      </c>
-      <c r="C468" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="469" spans="1:3">
       <c r="A469" t="s">
+        <v>867</v>
+      </c>
+      <c r="B469" t="s">
         <v>868</v>
       </c>
-      <c r="B469" t="s">
-        <v>869</v>
-      </c>
       <c r="C469" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="470" spans="1:3">
       <c r="A470" t="s">
+        <v>869</v>
+      </c>
+      <c r="B470" t="s">
         <v>870</v>
       </c>
-      <c r="B470" t="s">
-        <v>871</v>
-      </c>
       <c r="C470" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="471" spans="1:3">
       <c r="A471" t="s">
+        <v>871</v>
+      </c>
+      <c r="B471" t="s">
         <v>872</v>
       </c>
-      <c r="B471" t="s">
-        <v>873</v>
-      </c>
       <c r="C471" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="472" spans="1:3">
       <c r="A472" t="s">
+        <v>873</v>
+      </c>
+      <c r="B472" t="s">
         <v>874</v>
       </c>
-      <c r="B472" t="s">
-        <v>875</v>
-      </c>
       <c r="C472" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="473" spans="1:3">
       <c r="A473" t="s">
+        <v>875</v>
+      </c>
+      <c r="B473" t="s">
         <v>876</v>
       </c>
-      <c r="B473" t="s">
-        <v>877</v>
-      </c>
       <c r="C473" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="474" spans="1:3">
       <c r="A474" t="s">
+        <v>877</v>
+      </c>
+      <c r="B474" t="s">
         <v>878</v>
       </c>
-      <c r="B474" t="s">
-        <v>879</v>
-      </c>
       <c r="C474" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="475" spans="1:3">
       <c r="A475" t="s">
+        <v>879</v>
+      </c>
+      <c r="B475" t="s">
         <v>880</v>
       </c>
-      <c r="B475" t="s">
-        <v>881</v>
-      </c>
       <c r="C475" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="476" spans="1:3">
       <c r="A476" t="s">
+        <v>881</v>
+      </c>
+      <c r="B476" t="s">
         <v>882</v>
       </c>
-      <c r="B476" t="s">
-        <v>883</v>
-      </c>
       <c r="C476" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="477" spans="1:3">
       <c r="A477" t="s">
+        <v>883</v>
+      </c>
+      <c r="B477" t="s">
         <v>884</v>
       </c>
-      <c r="B477" t="s">
-        <v>885</v>
-      </c>
       <c r="C477" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="478" spans="1:3">
       <c r="A478" t="s">
+        <v>885</v>
+      </c>
+      <c r="B478" t="s">
         <v>886</v>
       </c>
-      <c r="B478" t="s">
-        <v>887</v>
-      </c>
       <c r="C478" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="479" spans="1:3">
       <c r="A479" t="s">
+        <v>887</v>
+      </c>
+      <c r="B479" t="s">
         <v>888</v>
       </c>
-      <c r="B479" t="s">
-        <v>889</v>
-      </c>
       <c r="C479" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="480" spans="1:3">
       <c r="A480" t="s">
+        <v>889</v>
+      </c>
+      <c r="B480" t="s">
         <v>890</v>
       </c>
-      <c r="B480" t="s">
-        <v>891</v>
-      </c>
       <c r="C480" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="481" spans="1:3">
       <c r="A481" t="s">
+        <v>891</v>
+      </c>
+      <c r="B481" t="s">
         <v>892</v>
       </c>
-      <c r="B481" t="s">
-        <v>893</v>
-      </c>
       <c r="C481" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="482" spans="1:3">
       <c r="A482" t="s">
+        <v>893</v>
+      </c>
+      <c r="B482" t="s">
         <v>894</v>
       </c>
-      <c r="B482" t="s">
-        <v>895</v>
-      </c>
       <c r="C482" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="483" spans="1:3">
       <c r="A483" t="s">
+        <v>895</v>
+      </c>
+      <c r="B483" t="s">
         <v>896</v>
       </c>
-      <c r="B483" t="s">
-        <v>897</v>
-      </c>
       <c r="C483" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="484" spans="1:3">
@@ -8889,7 +8886,7 @@
         <v>626</v>
       </c>
       <c r="C484" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="485" spans="1:3">
@@ -8900,7 +8897,7 @@
         <v>628</v>
       </c>
       <c r="C485" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="486" spans="1:3">
@@ -8911,7 +8908,7 @@
         <v>630</v>
       </c>
       <c r="C486" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="487" spans="1:3">
@@ -8922,7 +8919,7 @@
         <v>632</v>
       </c>
       <c r="C487" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="488" spans="1:3">
@@ -8933,7 +8930,7 @@
         <v>634</v>
       </c>
       <c r="C488" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="489" spans="1:3">
@@ -8944,183 +8941,183 @@
         <v>636</v>
       </c>
       <c r="C489" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="490" spans="1:3">
       <c r="A490" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B490" t="s">
         <v>1026</v>
       </c>
-      <c r="B490" t="s">
+      <c r="C490" t="s">
         <v>1027</v>
-      </c>
-      <c r="C490" t="s">
-        <v>1028</v>
       </c>
     </row>
     <row r="491" spans="1:3">
       <c r="A491" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B491" t="s">
         <v>1029</v>
       </c>
-      <c r="B491" t="s">
-        <v>1030</v>
-      </c>
       <c r="C491" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="492" spans="1:3">
       <c r="A492" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B492" t="s">
         <v>1031</v>
       </c>
-      <c r="B492" t="s">
-        <v>1032</v>
-      </c>
       <c r="C492" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="493" spans="1:3">
       <c r="A493" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B493" t="s">
         <v>1033</v>
       </c>
-      <c r="B493" t="s">
-        <v>1034</v>
-      </c>
       <c r="C493" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="494" spans="1:3">
       <c r="A494" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B494" t="s">
         <v>1035</v>
       </c>
-      <c r="B494" t="s">
-        <v>1036</v>
-      </c>
       <c r="C494" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="495" spans="1:3">
       <c r="A495" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B495" t="s">
         <v>1037</v>
       </c>
-      <c r="B495" t="s">
-        <v>1038</v>
-      </c>
       <c r="C495" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="496" spans="1:3">
       <c r="A496" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B496" t="s">
         <v>1039</v>
       </c>
-      <c r="B496" t="s">
-        <v>1040</v>
-      </c>
       <c r="C496" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="497" spans="1:3">
       <c r="A497" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B497" t="s">
         <v>1041</v>
       </c>
-      <c r="B497" t="s">
-        <v>1042</v>
-      </c>
       <c r="C497" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="498" spans="1:3">
       <c r="A498" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B498" t="s">
         <v>1043</v>
       </c>
-      <c r="B498" t="s">
-        <v>1044</v>
-      </c>
       <c r="C498" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="499" spans="1:3">
       <c r="A499" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B499" t="s">
         <v>1045</v>
       </c>
-      <c r="B499" t="s">
-        <v>1046</v>
-      </c>
       <c r="C499" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="500" spans="1:3">
       <c r="A500" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B500" t="s">
         <v>1047</v>
       </c>
-      <c r="B500" t="s">
-        <v>1048</v>
-      </c>
       <c r="C500" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="501" spans="1:3">
       <c r="A501" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B501" t="s">
         <v>1049</v>
       </c>
-      <c r="B501" t="s">
-        <v>1050</v>
-      </c>
       <c r="C501" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="502" spans="1:3">
       <c r="A502" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B502" t="s">
         <v>1051</v>
       </c>
-      <c r="B502" t="s">
-        <v>1052</v>
-      </c>
       <c r="C502" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="503" spans="1:3">
       <c r="A503" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B503" t="s">
         <v>1053</v>
       </c>
-      <c r="B503" t="s">
-        <v>1054</v>
-      </c>
       <c r="C503" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="504" spans="1:3">
       <c r="A504" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B504" t="s">
         <v>1055</v>
       </c>
-      <c r="B504" t="s">
-        <v>1056</v>
-      </c>
       <c r="C504" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="505" spans="1:3">
       <c r="A505" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B505" t="s">
         <v>1057</v>
       </c>
-      <c r="B505" t="s">
-        <v>1058</v>
-      </c>
       <c r="C505" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
03/06/2023 update. New major developments completed. 1. EBITDA margin and net profit margin added to metrics, long term debt to equity removed. 2. Business functions separated into different packages and interfaces. 3. Company titles can be updated automatically. 4. Some refactorings on variable names. 5. SonarLint issues fixed.
</commit_message>
<xml_diff>
--- a/src/main/resources/static/companies.xlsx
+++ b/src/main/resources/static/companies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\Development\Borsa-Istanbul\borsa-istanbul-backend\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C4DF10-930A-4A89-8998-B994219076B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606DEEBA-86F9-413C-90A4-457FBE687BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isyatirim" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="1057">
   <si>
     <t>BRSAN</t>
   </si>
@@ -1895,12 +1895,6 @@
   </si>
   <si>
     <t>Türk Hava Yolları</t>
-  </si>
-  <si>
-    <t>DOCO</t>
-  </si>
-  <si>
-    <t>DO &amp; CO Aktiengesellschaft</t>
   </si>
   <si>
     <t>GSDDE</t>
@@ -3553,10 +3547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C505"/>
+  <dimension ref="A1:C504"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C262" sqref="C262"/>
+    <sheetView tabSelected="1" topLeftCell="A470" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A484" sqref="A484:XFD484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3732,10 +3726,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="B16" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
@@ -3743,10 +3737,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="B17" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
@@ -3765,10 +3759,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="B19" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -3974,13 +3968,13 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
+        <v>771</v>
+      </c>
+      <c r="B38" t="s">
+        <v>772</v>
+      </c>
+      <c r="C38" t="s">
         <v>773</v>
-      </c>
-      <c r="B38" t="s">
-        <v>774</v>
-      </c>
-      <c r="C38" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -4266,7 +4260,7 @@
         <v>482</v>
       </c>
       <c r="C64" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -4277,7 +4271,7 @@
         <v>484</v>
       </c>
       <c r="C65" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -4288,7 +4282,7 @@
         <v>486</v>
       </c>
       <c r="C66" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -4299,7 +4293,7 @@
         <v>488</v>
       </c>
       <c r="C67" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -4310,7 +4304,7 @@
         <v>490</v>
       </c>
       <c r="C68" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -4321,7 +4315,7 @@
         <v>492</v>
       </c>
       <c r="C69" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -4332,7 +4326,7 @@
         <v>494</v>
       </c>
       <c r="C70" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -4343,7 +4337,7 @@
         <v>496</v>
       </c>
       <c r="C71" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -4354,7 +4348,7 @@
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -4365,7 +4359,7 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -4376,7 +4370,7 @@
         <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -4387,7 +4381,7 @@
         <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -4398,7 +4392,7 @@
         <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -4409,7 +4403,7 @@
         <v>11</v>
       </c>
       <c r="C77" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -4420,7 +4414,7 @@
         <v>13</v>
       </c>
       <c r="C78" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -4431,7 +4425,7 @@
         <v>15</v>
       </c>
       <c r="C79" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -4442,7 +4436,7 @@
         <v>17</v>
       </c>
       <c r="C80" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -4453,7 +4447,7 @@
         <v>19</v>
       </c>
       <c r="C81" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -4464,7 +4458,7 @@
         <v>21</v>
       </c>
       <c r="C82" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -4475,7 +4469,7 @@
         <v>23</v>
       </c>
       <c r="C83" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -4524,57 +4518,57 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
+        <v>975</v>
+      </c>
+      <c r="B88" t="s">
+        <v>976</v>
+      </c>
+      <c r="C88" t="s">
         <v>977</v>
-      </c>
-      <c r="B88" t="s">
-        <v>978</v>
-      </c>
-      <c r="C88" t="s">
-        <v>979</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="B89" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="C89" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B90" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="C90" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B91" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="C91" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
+        <v>985</v>
+      </c>
+      <c r="B92" t="s">
+        <v>986</v>
+      </c>
+      <c r="C92" t="s">
         <v>987</v>
-      </c>
-      <c r="B92" t="s">
-        <v>988</v>
-      </c>
-      <c r="C92" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -4601,10 +4595,10 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="B95" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="C95" t="s">
         <v>102</v>
@@ -4733,10 +4727,10 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="B107" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="C107" t="s">
         <v>102</v>
@@ -4975,10 +4969,10 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="B129" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>102</v>
@@ -4992,18 +4986,18 @@
         <v>507</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="B131" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -5014,18 +5008,18 @@
         <v>509</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B133" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -5036,7 +5030,7 @@
         <v>511</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -5047,7 +5041,7 @@
         <v>513</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -5058,7 +5052,7 @@
         <v>515</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -5066,7 +5060,7 @@
         <v>169</v>
       </c>
       <c r="B137" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="C137" t="s">
         <v>170</v>
@@ -5074,10 +5068,10 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B138" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C138" t="s">
         <v>170</v>
@@ -5113,7 +5107,7 @@
         <v>517</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -5124,7 +5118,7 @@
         <v>519</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -5135,7 +5129,7 @@
         <v>521</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -5146,7 +5140,7 @@
         <v>523</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -5157,7 +5151,7 @@
         <v>525</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -5168,7 +5162,7 @@
         <v>527</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -5179,7 +5173,7 @@
         <v>529</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -5190,7 +5184,7 @@
         <v>531</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -5201,7 +5195,7 @@
         <v>533</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -5217,10 +5211,10 @@
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="B151" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C151" t="s">
         <v>177</v>
@@ -5261,10 +5255,10 @@
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B155" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C155" t="s">
         <v>177</v>
@@ -5316,10 +5310,10 @@
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="B160" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="C160" t="s">
         <v>177</v>
@@ -5338,10 +5332,10 @@
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="B162" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="C162" t="s">
         <v>177</v>
@@ -6026,7 +6020,7 @@
         <v>618</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -6037,7 +6031,7 @@
         <v>620</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -6048,7 +6042,7 @@
         <v>622</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -6059,29 +6053,29 @@
         <v>624</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
+        <v>920</v>
+      </c>
+      <c r="B228" t="s">
+        <v>921</v>
+      </c>
+      <c r="C228" t="s">
         <v>922</v>
-      </c>
-      <c r="B228" t="s">
-        <v>923</v>
-      </c>
-      <c r="C228" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="B229" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C229" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -6092,7 +6086,7 @@
         <v>235</v>
       </c>
       <c r="C230" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -6103,7 +6097,7 @@
         <v>237</v>
       </c>
       <c r="C231" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -6114,7 +6108,7 @@
         <v>239</v>
       </c>
       <c r="C232" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -6125,7 +6119,7 @@
         <v>241</v>
       </c>
       <c r="C233" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -6136,7 +6130,7 @@
         <v>243</v>
       </c>
       <c r="C234" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -6147,7 +6141,7 @@
         <v>245</v>
       </c>
       <c r="C235" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -6158,7 +6152,7 @@
         <v>247</v>
       </c>
       <c r="C236" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -6169,7 +6163,7 @@
         <v>249</v>
       </c>
       <c r="C237" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -6180,7 +6174,7 @@
         <v>251</v>
       </c>
       <c r="C238" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -6191,7 +6185,7 @@
         <v>253</v>
       </c>
       <c r="C239" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -6202,7 +6196,7 @@
         <v>255</v>
       </c>
       <c r="C240" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -6213,7 +6207,7 @@
         <v>257</v>
       </c>
       <c r="C241" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -6224,7 +6218,7 @@
         <v>259</v>
       </c>
       <c r="C242" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -6235,7 +6229,7 @@
         <v>261</v>
       </c>
       <c r="C243" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -6246,7 +6240,7 @@
         <v>263</v>
       </c>
       <c r="C244" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -6257,7 +6251,7 @@
         <v>265</v>
       </c>
       <c r="C245" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -6268,7 +6262,7 @@
         <v>267</v>
       </c>
       <c r="C246" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -6279,7 +6273,7 @@
         <v>269</v>
       </c>
       <c r="C247" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -6290,7 +6284,7 @@
         <v>271</v>
       </c>
       <c r="C248" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -6301,7 +6295,7 @@
         <v>273</v>
       </c>
       <c r="C249" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -6312,7 +6306,7 @@
         <v>275</v>
       </c>
       <c r="C250" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -6323,7 +6317,7 @@
         <v>277</v>
       </c>
       <c r="C251" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -6334,7 +6328,7 @@
         <v>279</v>
       </c>
       <c r="C252" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -6345,7 +6339,7 @@
         <v>281</v>
       </c>
       <c r="C253" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -6356,7 +6350,7 @@
         <v>283</v>
       </c>
       <c r="C254" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -6367,7 +6361,7 @@
         <v>285</v>
       </c>
       <c r="C255" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -6378,7 +6372,7 @@
         <v>287</v>
       </c>
       <c r="C256" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -6389,7 +6383,7 @@
         <v>289</v>
       </c>
       <c r="C257" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -6400,7 +6394,7 @@
         <v>291</v>
       </c>
       <c r="C258" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -6411,7 +6405,7 @@
         <v>293</v>
       </c>
       <c r="C259" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -6422,7 +6416,7 @@
         <v>295</v>
       </c>
       <c r="C260" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="261" spans="1:3">
@@ -6433,92 +6427,92 @@
         <v>297</v>
       </c>
       <c r="C261" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
+        <v>774</v>
+      </c>
+      <c r="B262" t="s">
+        <v>775</v>
+      </c>
+      <c r="C262" t="s">
         <v>776</v>
-      </c>
-      <c r="B262" t="s">
-        <v>777</v>
-      </c>
-      <c r="C262" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="B263" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C263" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="B264" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C264" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B265" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C265" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" t="s">
+        <v>895</v>
+      </c>
+      <c r="B266" t="s">
+        <v>896</v>
+      </c>
+      <c r="C266" t="s">
         <v>897</v>
-      </c>
-      <c r="B266" t="s">
-        <v>898</v>
-      </c>
-      <c r="C266" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="B267" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="C267" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="B268" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="C268" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="B269" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>318</v>
@@ -6581,354 +6575,354 @@
     </row>
     <row r="275" spans="1:3">
       <c r="A275" t="s">
+        <v>783</v>
+      </c>
+      <c r="B275" t="s">
+        <v>784</v>
+      </c>
+      <c r="C275" t="s">
         <v>785</v>
-      </c>
-      <c r="B275" t="s">
-        <v>786</v>
-      </c>
-      <c r="C275" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="276" spans="1:3">
       <c r="A276" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B276" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C276" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="277" spans="1:3">
       <c r="A277" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B277" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C277" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="278" spans="1:3">
       <c r="A278" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B278" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="C278" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B279" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C279" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="280" spans="1:3">
       <c r="A280" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B280" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C280" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="281" spans="1:3">
       <c r="A281" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B281" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="C281" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="282" spans="1:3">
       <c r="A282" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B282" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="C282" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B283" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="C283" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="284" spans="1:3">
       <c r="A284" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B284" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C284" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="285" spans="1:3">
       <c r="A285" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B285" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C285" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="286" spans="1:3">
       <c r="A286" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B286" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="C286" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="287" spans="1:3">
       <c r="A287" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B287" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="C287" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="288" spans="1:3">
       <c r="A288" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B288" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="C288" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="289" spans="1:3">
       <c r="A289" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B289" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="C289" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="290" spans="1:3">
       <c r="A290" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B290" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C290" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="291" spans="1:3">
       <c r="A291" t="s">
+        <v>927</v>
+      </c>
+      <c r="B291" t="s">
+        <v>928</v>
+      </c>
+      <c r="C291" t="s">
         <v>929</v>
-      </c>
-      <c r="B291" t="s">
-        <v>930</v>
-      </c>
-      <c r="C291" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="292" spans="1:3">
       <c r="A292" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="B292" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="C292" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="293" spans="1:3">
       <c r="A293" t="s">
+        <v>731</v>
+      </c>
+      <c r="B293" t="s">
+        <v>732</v>
+      </c>
+      <c r="C293" t="s">
         <v>733</v>
-      </c>
-      <c r="B293" t="s">
-        <v>734</v>
-      </c>
-      <c r="C293" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="294" spans="1:3">
       <c r="A294" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B294" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="C294" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="295" spans="1:3">
       <c r="A295" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B295" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C295" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="296" spans="1:3">
       <c r="A296" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B296" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C296" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="297" spans="1:3">
       <c r="A297" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B297" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C297" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="298" spans="1:3">
       <c r="A298" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B298" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C298" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="299" spans="1:3">
       <c r="A299" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B299" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C299" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="300" spans="1:3">
       <c r="A300" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B300" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C300" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="301" spans="1:3">
       <c r="A301" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B301" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C301" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="302" spans="1:3">
       <c r="A302" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B302" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C302" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="303" spans="1:3">
       <c r="A303" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B303" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C303" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="304" spans="1:3">
       <c r="A304" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B304" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="C304" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="305" spans="1:3">
       <c r="A305" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B305" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C305" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="306" spans="1:3">
       <c r="A306" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B306" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C306" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="307" spans="1:3">
@@ -7109,167 +7103,167 @@
     </row>
     <row r="323" spans="1:3">
       <c r="A323" t="s">
+        <v>932</v>
+      </c>
+      <c r="B323" t="s">
+        <v>933</v>
+      </c>
+      <c r="C323" t="s">
         <v>934</v>
-      </c>
-      <c r="B323" t="s">
-        <v>935</v>
-      </c>
-      <c r="C323" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="324" spans="1:3">
       <c r="A324" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="B324" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="C324" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="325" spans="1:3">
       <c r="A325" t="s">
+        <v>760</v>
+      </c>
+      <c r="B325" t="s">
+        <v>761</v>
+      </c>
+      <c r="C325" t="s">
         <v>762</v>
-      </c>
-      <c r="B325" t="s">
-        <v>763</v>
-      </c>
-      <c r="C325" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="326" spans="1:3">
       <c r="A326" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B326" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="C326" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="327" spans="1:3">
       <c r="A327" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B327" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C327" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="328" spans="1:3">
       <c r="A328" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B328" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C328" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="329" spans="1:3">
       <c r="A329" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="B329" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C329" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="330" spans="1:3">
       <c r="A330" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B330" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C330" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="331" spans="1:3">
       <c r="A331" t="s">
+        <v>937</v>
+      </c>
+      <c r="B331" t="s">
+        <v>938</v>
+      </c>
+      <c r="C331" t="s">
         <v>939</v>
-      </c>
-      <c r="B331" t="s">
-        <v>940</v>
-      </c>
-      <c r="C331" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="332" spans="1:3">
       <c r="A332" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="B332" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C332" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="333" spans="1:3">
       <c r="A333" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="B333" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="C333" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="334" spans="1:3">
       <c r="A334" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="B334" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="C334" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="335" spans="1:3">
       <c r="A335" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="B335" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="C335" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="336" spans="1:3">
       <c r="A336" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="B336" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="C336" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="337" spans="1:3">
       <c r="A337" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="B337" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="C337" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="338" spans="1:3">
@@ -7280,7 +7274,7 @@
         <v>299</v>
       </c>
       <c r="C338" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="339" spans="1:3">
@@ -7291,7 +7285,7 @@
         <v>301</v>
       </c>
       <c r="C339" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="340" spans="1:3">
@@ -7302,7 +7296,7 @@
         <v>303</v>
       </c>
       <c r="C340" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="341" spans="1:3">
@@ -7313,7 +7307,7 @@
         <v>305</v>
       </c>
       <c r="C341" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="342" spans="1:3">
@@ -7324,7 +7318,7 @@
         <v>307</v>
       </c>
       <c r="C342" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="343" spans="1:3">
@@ -7335,7 +7329,7 @@
         <v>309</v>
       </c>
       <c r="C343" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="344" spans="1:3">
@@ -7346,7 +7340,7 @@
         <v>311</v>
       </c>
       <c r="C344" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="345" spans="1:3">
@@ -7357,7 +7351,7 @@
         <v>313</v>
       </c>
       <c r="C345" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="346" spans="1:3">
@@ -7368,73 +7362,73 @@
         <v>315</v>
       </c>
       <c r="C346" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="347" spans="1:3">
       <c r="A347" t="s">
+        <v>954</v>
+      </c>
+      <c r="B347" t="s">
+        <v>955</v>
+      </c>
+      <c r="C347" t="s">
         <v>956</v>
-      </c>
-      <c r="B347" t="s">
-        <v>957</v>
-      </c>
-      <c r="C347" t="s">
-        <v>958</v>
       </c>
     </row>
     <row r="348" spans="1:3">
       <c r="A348" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="B348" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C348" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="349" spans="1:3">
       <c r="A349" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="B349" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C349" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="350" spans="1:3">
       <c r="A350" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B350" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="C350" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="351" spans="1:3">
       <c r="A351" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="B351" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="C351" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="352" spans="1:3">
       <c r="A352" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="B352" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="C352" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="353" spans="1:3">
@@ -7527,167 +7521,167 @@
     </row>
     <row r="361" spans="1:3">
       <c r="A361" t="s">
+        <v>992</v>
+      </c>
+      <c r="B361" t="s">
+        <v>993</v>
+      </c>
+      <c r="C361" t="s">
         <v>994</v>
-      </c>
-      <c r="B361" t="s">
-        <v>995</v>
-      </c>
-      <c r="C361" t="s">
-        <v>996</v>
       </c>
     </row>
     <row r="362" spans="1:3">
       <c r="A362" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="B362" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="C362" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="363" spans="1:3">
       <c r="A363" t="s">
+        <v>816</v>
+      </c>
+      <c r="B363" t="s">
+        <v>817</v>
+      </c>
+      <c r="C363" t="s">
         <v>818</v>
-      </c>
-      <c r="B363" t="s">
-        <v>819</v>
-      </c>
-      <c r="C363" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="364" spans="1:3">
       <c r="A364" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B364" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C364" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="365" spans="1:3">
       <c r="A365" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B365" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="C365" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="366" spans="1:3">
       <c r="A366" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B366" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="C366" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="367" spans="1:3">
       <c r="A367" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B367" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="C367" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="368" spans="1:3">
       <c r="A368" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B368" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C368" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="369" spans="1:3">
       <c r="A369" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B369" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C369" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="370" spans="1:3">
       <c r="A370" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B370" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="C370" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="371" spans="1:3">
       <c r="A371" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B371" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="C371" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="372" spans="1:3">
       <c r="A372" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B372" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="C372" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="373" spans="1:3">
       <c r="A373" t="s">
+        <v>997</v>
+      </c>
+      <c r="B373" t="s">
+        <v>998</v>
+      </c>
+      <c r="C373" t="s">
         <v>999</v>
-      </c>
-      <c r="B373" t="s">
-        <v>1000</v>
-      </c>
-      <c r="C373" t="s">
-        <v>1001</v>
       </c>
     </row>
     <row r="374" spans="1:3">
       <c r="A374" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="B374" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C374" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="375" spans="1:3">
       <c r="A375" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="B375" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="C375" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="376" spans="1:3">
@@ -7698,7 +7692,7 @@
         <v>378</v>
       </c>
       <c r="C376" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="377" spans="1:3">
@@ -7709,7 +7703,7 @@
         <v>380</v>
       </c>
       <c r="C377" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="378" spans="1:3">
@@ -7720,7 +7714,7 @@
         <v>382</v>
       </c>
       <c r="C378" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="379" spans="1:3">
@@ -7731,7 +7725,7 @@
         <v>384</v>
       </c>
       <c r="C379" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="380" spans="1:3">
@@ -7742,7 +7736,7 @@
         <v>386</v>
       </c>
       <c r="C380" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="381" spans="1:3">
@@ -7753,18 +7747,18 @@
         <v>388</v>
       </c>
       <c r="C381" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="382" spans="1:3">
       <c r="A382" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="B382" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="C382" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="383" spans="1:3">
@@ -7775,7 +7769,7 @@
         <v>390</v>
       </c>
       <c r="C383" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="384" spans="1:3">
@@ -7786,7 +7780,7 @@
         <v>392</v>
       </c>
       <c r="C384" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="385" spans="1:3">
@@ -7797,7 +7791,7 @@
         <v>394</v>
       </c>
       <c r="C385" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="386" spans="1:3">
@@ -7808,7 +7802,7 @@
         <v>396</v>
       </c>
       <c r="C386" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="387" spans="1:3">
@@ -7819,7 +7813,7 @@
         <v>398</v>
       </c>
       <c r="C387" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="388" spans="1:3">
@@ -7830,425 +7824,425 @@
         <v>400</v>
       </c>
       <c r="C388" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="389" spans="1:3">
       <c r="A389" t="s">
+        <v>635</v>
+      </c>
+      <c r="B389" t="s">
+        <v>636</v>
+      </c>
+      <c r="C389" t="s">
         <v>637</v>
-      </c>
-      <c r="B389" t="s">
-        <v>638</v>
-      </c>
-      <c r="C389" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="390" spans="1:3">
       <c r="A390" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B390" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C390" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="391" spans="1:3">
       <c r="A391" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B391" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C391" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="392" spans="1:3">
       <c r="A392" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B392" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C392" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="393" spans="1:3">
       <c r="A393" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B393" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C393" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="394" spans="1:3">
       <c r="A394" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B394" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C394" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="395" spans="1:3">
       <c r="A395" t="s">
+        <v>837</v>
+      </c>
+      <c r="B395" t="s">
+        <v>838</v>
+      </c>
+      <c r="C395" t="s">
         <v>839</v>
-      </c>
-      <c r="B395" t="s">
-        <v>840</v>
-      </c>
-      <c r="C395" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="396" spans="1:3">
       <c r="A396" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B396" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="C396" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="397" spans="1:3">
       <c r="A397" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="B397" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C397" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="398" spans="1:3">
       <c r="A398" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B398" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C398" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="399" spans="1:3">
       <c r="A399" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B399" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C399" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="400" spans="1:3">
       <c r="A400" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="B400" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="C400" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="401" spans="1:3">
       <c r="A401" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B401" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="C401" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="402" spans="1:3">
       <c r="A402" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="B402" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C402" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="403" spans="1:3">
       <c r="A403" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="B403" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="C403" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="404" spans="1:3">
       <c r="A404" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="B404" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="C404" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="405" spans="1:3">
       <c r="A405" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B405" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="C405" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="406" spans="1:3">
       <c r="A406" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B406" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="C406" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="407" spans="1:3">
       <c r="A407" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B407" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C407" t="s">
         <v>1009</v>
-      </c>
-      <c r="B407" t="s">
-        <v>1010</v>
-      </c>
-      <c r="C407" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="408" spans="1:3">
       <c r="A408" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="B408" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="C408" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="409" spans="1:3">
       <c r="A409" t="s">
+        <v>663</v>
+      </c>
+      <c r="B409" t="s">
+        <v>664</v>
+      </c>
+      <c r="C409" t="s">
         <v>665</v>
-      </c>
-      <c r="B409" t="s">
-        <v>666</v>
-      </c>
-      <c r="C409" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="410" spans="1:3">
       <c r="A410" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B410" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C410" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="411" spans="1:3">
       <c r="A411" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B411" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C411" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="412" spans="1:3">
       <c r="A412" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B412" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C412" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="413" spans="1:3">
       <c r="A413" t="s">
+        <v>648</v>
+      </c>
+      <c r="B413" t="s">
+        <v>649</v>
+      </c>
+      <c r="C413" t="s">
         <v>650</v>
-      </c>
-      <c r="B413" t="s">
-        <v>651</v>
-      </c>
-      <c r="C413" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="414" spans="1:3">
       <c r="A414" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B414" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C414" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="415" spans="1:3">
       <c r="A415" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B415" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C415" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="416" spans="1:3">
       <c r="A416" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B416" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C416" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="417" spans="1:3">
       <c r="A417" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B417" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C417" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="418" spans="1:3">
       <c r="A418" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B418" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C418" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="419" spans="1:3">
       <c r="A419" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B419" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C419" t="s">
         <v>1014</v>
-      </c>
-      <c r="B419" t="s">
-        <v>1015</v>
-      </c>
-      <c r="C419" t="s">
-        <v>1016</v>
       </c>
     </row>
     <row r="420" spans="1:3">
       <c r="A420" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="B420" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="C420" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="421" spans="1:3">
       <c r="A421" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="B421" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="C421" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="422" spans="1:3">
       <c r="A422" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="B422" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="C422" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="423" spans="1:3">
       <c r="A423" t="s">
+        <v>672</v>
+      </c>
+      <c r="B423" t="s">
+        <v>673</v>
+      </c>
+      <c r="C423" t="s">
         <v>674</v>
-      </c>
-      <c r="B423" t="s">
-        <v>675</v>
-      </c>
-      <c r="C423" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="424" spans="1:3">
       <c r="A424" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B424" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C424" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="425" spans="1:3">
       <c r="A425" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B425" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C425" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="426" spans="1:3">
       <c r="A426" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B426" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C426" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="427" spans="1:3">
@@ -8429,453 +8423,453 @@
     </row>
     <row r="443" spans="1:3">
       <c r="A443" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B443" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C443" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="444" spans="1:3">
       <c r="A444" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B444" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C444" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="445" spans="1:3">
       <c r="A445" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B445" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C445" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="446" spans="1:3">
       <c r="A446" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B446" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C446" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="447" spans="1:3">
       <c r="A447" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B447" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C447" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="448" spans="1:3">
       <c r="A448" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B448" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C448" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="449" spans="1:3">
       <c r="A449" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B449" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C449" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="450" spans="1:3">
       <c r="A450" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B450" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C450" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="451" spans="1:3">
       <c r="A451" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B451" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C451" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="452" spans="1:3">
       <c r="A452" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B452" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C452" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="453" spans="1:3">
       <c r="A453" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B453" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C453" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="454" spans="1:3">
       <c r="A454" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B454" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C454" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="455" spans="1:3">
       <c r="A455" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B455" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C455" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="456" spans="1:3">
       <c r="A456" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B456" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C456" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="457" spans="1:3">
       <c r="A457" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B457" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C457" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="458" spans="1:3">
       <c r="A458" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B458" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="C458" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="459" spans="1:3">
       <c r="A459" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B459" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="C459" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="460" spans="1:3">
       <c r="A460" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B460" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="C460" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="461" spans="1:3">
       <c r="A461" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B461" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C461" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="462" spans="1:3">
       <c r="A462" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B462" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C462" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="463" spans="1:3">
       <c r="A463" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B463" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C463" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="464" spans="1:3">
       <c r="A464" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B464" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C464" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="465" spans="1:3">
       <c r="A465" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B465" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C465" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="466" spans="1:3">
       <c r="A466" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B466" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C466" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="467" spans="1:3">
       <c r="A467" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B467" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C467" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="468" spans="1:3">
       <c r="A468" t="s">
+        <v>862</v>
+      </c>
+      <c r="B468" t="s">
+        <v>863</v>
+      </c>
+      <c r="C468" t="s">
         <v>864</v>
-      </c>
-      <c r="B468" t="s">
-        <v>865</v>
-      </c>
-      <c r="C468" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="469" spans="1:3">
       <c r="A469" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="B469" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="C469" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="470" spans="1:3">
       <c r="A470" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B470" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="C470" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="471" spans="1:3">
       <c r="A471" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B471" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C471" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="472" spans="1:3">
       <c r="A472" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="B472" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="C472" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="473" spans="1:3">
       <c r="A473" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B473" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="C473" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="474" spans="1:3">
       <c r="A474" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B474" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="C474" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="475" spans="1:3">
       <c r="A475" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="B475" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="C475" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="476" spans="1:3">
       <c r="A476" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="B476" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="C476" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="477" spans="1:3">
       <c r="A477" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B477" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="C477" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="478" spans="1:3">
       <c r="A478" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B478" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="C478" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="479" spans="1:3">
       <c r="A479" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="B479" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="C479" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="480" spans="1:3">
       <c r="A480" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B480" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="C480" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="481" spans="1:3">
       <c r="A481" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="B481" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C481" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="482" spans="1:3">
       <c r="A482" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="B482" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="C482" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="483" spans="1:3">
       <c r="A483" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="B483" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="C483" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="484" spans="1:3">
@@ -8886,7 +8880,7 @@
         <v>626</v>
       </c>
       <c r="C484" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="485" spans="1:3">
@@ -8897,7 +8891,7 @@
         <v>628</v>
       </c>
       <c r="C485" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="486" spans="1:3">
@@ -8908,7 +8902,7 @@
         <v>630</v>
       </c>
       <c r="C486" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="487" spans="1:3">
@@ -8919,7 +8913,7 @@
         <v>632</v>
       </c>
       <c r="C487" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="488" spans="1:3">
@@ -8930,29 +8924,29 @@
         <v>634</v>
       </c>
       <c r="C488" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="489" spans="1:3">
       <c r="A489" t="s">
-        <v>635</v>
+        <v>1023</v>
       </c>
       <c r="B489" t="s">
-        <v>636</v>
+        <v>1024</v>
       </c>
       <c r="C489" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="490" spans="1:3">
       <c r="A490" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B490" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C490" t="s">
         <v>1025</v>
-      </c>
-      <c r="B490" t="s">
-        <v>1026</v>
-      </c>
-      <c r="C490" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="491" spans="1:3">
@@ -8963,7 +8957,7 @@
         <v>1029</v>
       </c>
       <c r="C491" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="492" spans="1:3">
@@ -8974,7 +8968,7 @@
         <v>1031</v>
       </c>
       <c r="C492" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="493" spans="1:3">
@@ -8985,7 +8979,7 @@
         <v>1033</v>
       </c>
       <c r="C493" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="494" spans="1:3">
@@ -8996,7 +8990,7 @@
         <v>1035</v>
       </c>
       <c r="C494" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="495" spans="1:3">
@@ -9007,7 +9001,7 @@
         <v>1037</v>
       </c>
       <c r="C495" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="496" spans="1:3">
@@ -9018,7 +9012,7 @@
         <v>1039</v>
       </c>
       <c r="C496" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="497" spans="1:3">
@@ -9029,7 +9023,7 @@
         <v>1041</v>
       </c>
       <c r="C497" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="498" spans="1:3">
@@ -9040,7 +9034,7 @@
         <v>1043</v>
       </c>
       <c r="C498" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="499" spans="1:3">
@@ -9051,7 +9045,7 @@
         <v>1045</v>
       </c>
       <c r="C499" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="500" spans="1:3">
@@ -9062,7 +9056,7 @@
         <v>1047</v>
       </c>
       <c r="C500" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="501" spans="1:3">
@@ -9073,7 +9067,7 @@
         <v>1049</v>
       </c>
       <c r="C501" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="502" spans="1:3">
@@ -9084,7 +9078,7 @@
         <v>1051</v>
       </c>
       <c r="C502" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="503" spans="1:3">
@@ -9095,7 +9089,7 @@
         <v>1053</v>
       </c>
       <c r="C503" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="504" spans="1:3">
@@ -9106,23 +9100,12 @@
         <v>1055</v>
       </c>
       <c r="C504" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="505" spans="1:3">
-      <c r="A505" t="s">
-        <v>1056</v>
-      </c>
-      <c r="B505" t="s">
-        <v>1057</v>
-      </c>
-      <c r="C505" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C505">
-    <sortCondition ref="C1:C505"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C504">
+    <sortCondition ref="C1:C504"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
04/06/2023 commit. Minor optimizations.
</commit_message>
<xml_diff>
--- a/src/main/resources/static/companies.xlsx
+++ b/src/main/resources/static/companies.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\Development\Borsa-Istanbul\borsa-istanbul-backend\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606DEEBA-86F9-413C-90A4-457FBE687BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765EB471-6B8E-4F18-B481-6769D1721423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isyatirim" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="1057">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="1059">
   <si>
     <t>BRSAN</t>
   </si>
@@ -3191,6 +3204,12 @@
   </si>
   <si>
     <t>Elektrik Makineleri Üretimi</t>
+  </si>
+  <si>
+    <t>UMPAS</t>
+  </si>
+  <si>
+    <t>Umpaş Holding</t>
   </si>
 </sst>
 </file>
@@ -3547,10 +3566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C504"/>
+  <dimension ref="A1:C505"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A470" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A484" sqref="A484:XFD484"/>
+    <sheetView tabSelected="1" topLeftCell="A244" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F257" sqref="F257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5244,10 +5263,10 @@
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>182</v>
+        <v>914</v>
       </c>
       <c r="B154" t="s">
-        <v>183</v>
+        <v>915</v>
       </c>
       <c r="C154" t="s">
         <v>177</v>
@@ -5255,10 +5274,10 @@
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>914</v>
+        <v>184</v>
       </c>
       <c r="B155" t="s">
-        <v>915</v>
+        <v>185</v>
       </c>
       <c r="C155" t="s">
         <v>177</v>
@@ -5266,10 +5285,10 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B156" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C156" t="s">
         <v>177</v>
@@ -5277,10 +5296,10 @@
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B157" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C157" t="s">
         <v>177</v>
@@ -5288,10 +5307,10 @@
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B158" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C158" t="s">
         <v>177</v>
@@ -5299,10 +5318,10 @@
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>190</v>
+        <v>916</v>
       </c>
       <c r="B159" t="s">
-        <v>191</v>
+        <v>917</v>
       </c>
       <c r="C159" t="s">
         <v>177</v>
@@ -5310,10 +5329,10 @@
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>916</v>
+        <v>192</v>
       </c>
       <c r="B160" t="s">
-        <v>917</v>
+        <v>193</v>
       </c>
       <c r="C160" t="s">
         <v>177</v>
@@ -5321,10 +5340,10 @@
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>192</v>
+        <v>918</v>
       </c>
       <c r="B161" t="s">
-        <v>193</v>
+        <v>919</v>
       </c>
       <c r="C161" t="s">
         <v>177</v>
@@ -5332,10 +5351,10 @@
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>918</v>
+        <v>194</v>
       </c>
       <c r="B162" t="s">
-        <v>919</v>
+        <v>195</v>
       </c>
       <c r="C162" t="s">
         <v>177</v>
@@ -5343,10 +5362,10 @@
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B163" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C163" t="s">
         <v>177</v>
@@ -5354,10 +5373,10 @@
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B164" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C164" t="s">
         <v>177</v>
@@ -5365,10 +5384,10 @@
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B165" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C165" t="s">
         <v>177</v>
@@ -5376,10 +5395,10 @@
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B166" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C166" t="s">
         <v>177</v>
@@ -5387,10 +5406,10 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B167" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C167" t="s">
         <v>177</v>
@@ -5398,10 +5417,10 @@
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B168" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C168" t="s">
         <v>177</v>
@@ -5409,10 +5428,10 @@
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B169" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C169" t="s">
         <v>177</v>
@@ -5420,10 +5439,10 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B170" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C170" t="s">
         <v>177</v>
@@ -5431,10 +5450,10 @@
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B171" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C171" t="s">
         <v>177</v>
@@ -5442,10 +5461,10 @@
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B172" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C172" t="s">
         <v>177</v>
@@ -5453,10 +5472,10 @@
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B173" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C173" t="s">
         <v>177</v>
@@ -5464,10 +5483,10 @@
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B174" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C174" t="s">
         <v>177</v>
@@ -5475,10 +5494,10 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B175" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C175" t="s">
         <v>177</v>
@@ -5486,10 +5505,10 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B176" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C176" t="s">
         <v>177</v>
@@ -5497,10 +5516,10 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B177" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C177" t="s">
         <v>177</v>
@@ -5508,10 +5527,10 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B178" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C178" t="s">
         <v>177</v>
@@ -5519,10 +5538,10 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B179" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C179" t="s">
         <v>177</v>
@@ -5530,10 +5549,10 @@
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B180" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C180" t="s">
         <v>177</v>
@@ -5541,10 +5560,10 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B181" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C181" t="s">
         <v>177</v>
@@ -5552,21 +5571,21 @@
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>232</v>
+        <v>534</v>
       </c>
       <c r="B182" t="s">
-        <v>233</v>
+        <v>535</v>
       </c>
       <c r="C182" t="s">
-        <v>177</v>
+        <v>536</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="B183" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="C183" t="s">
         <v>536</v>
@@ -5574,10 +5593,10 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B184" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C184" t="s">
         <v>536</v>
@@ -5585,10 +5604,10 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="B185" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="C185" t="s">
         <v>536</v>
@@ -5596,10 +5615,10 @@
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B186" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="C186" t="s">
         <v>536</v>
@@ -5607,10 +5626,10 @@
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B187" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C187" t="s">
         <v>536</v>
@@ -5618,10 +5637,10 @@
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B188" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="C188" t="s">
         <v>536</v>
@@ -5629,10 +5648,10 @@
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B189" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="C189" t="s">
         <v>536</v>
@@ -5640,10 +5659,10 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B190" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C190" t="s">
         <v>536</v>
@@ -5651,10 +5670,10 @@
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="B191" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="C191" t="s">
         <v>536</v>
@@ -5662,10 +5681,10 @@
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="B192" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="C192" t="s">
         <v>536</v>
@@ -5673,10 +5692,10 @@
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B193" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C193" t="s">
         <v>536</v>
@@ -5684,10 +5703,10 @@
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="B194" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="C194" t="s">
         <v>536</v>
@@ -5695,10 +5714,10 @@
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="B195" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C195" t="s">
         <v>536</v>
@@ -5706,10 +5725,10 @@
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B196" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="C196" t="s">
         <v>536</v>
@@ -5717,10 +5736,10 @@
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="B197" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="C197" t="s">
         <v>536</v>
@@ -5728,10 +5747,10 @@
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="B198" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="C198" t="s">
         <v>536</v>
@@ -5739,10 +5758,10 @@
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="B199" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="C199" t="s">
         <v>536</v>
@@ -5750,10 +5769,10 @@
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="B200" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="C200" t="s">
         <v>536</v>
@@ -5761,10 +5780,10 @@
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="B201" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C201" t="s">
         <v>536</v>
@@ -5772,10 +5791,10 @@
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B202" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C202" t="s">
         <v>536</v>
@@ -5783,10 +5802,10 @@
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="B203" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="C203" t="s">
         <v>536</v>
@@ -5794,10 +5813,10 @@
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="B204" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C204" t="s">
         <v>536</v>
@@ -5805,10 +5824,10 @@
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="B205" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C205" t="s">
         <v>536</v>
@@ -5816,10 +5835,10 @@
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="B206" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C206" t="s">
         <v>536</v>
@@ -5827,10 +5846,10 @@
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="B207" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="C207" t="s">
         <v>536</v>
@@ -5838,10 +5857,10 @@
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="B208" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="C208" t="s">
         <v>536</v>
@@ -5849,10 +5868,10 @@
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="B209" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="C209" t="s">
         <v>536</v>
@@ -5860,10 +5879,10 @@
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="B210" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C210" t="s">
         <v>536</v>
@@ -5871,10 +5890,10 @@
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="B211" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C211" t="s">
         <v>536</v>
@@ -5882,10 +5901,10 @@
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="B212" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="C212" t="s">
         <v>536</v>
@@ -5893,10 +5912,10 @@
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="B213" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="C213" t="s">
         <v>536</v>
@@ -5904,10 +5923,10 @@
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="B214" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="C214" t="s">
         <v>536</v>
@@ -5915,10 +5934,10 @@
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="B215" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="C215" t="s">
         <v>536</v>
@@ -5926,10 +5945,10 @@
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="B216" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="C216" t="s">
         <v>536</v>
@@ -5937,10 +5956,10 @@
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="B217" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C217" t="s">
         <v>536</v>
@@ -5948,10 +5967,10 @@
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="B218" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="C218" t="s">
         <v>536</v>
@@ -5959,10 +5978,10 @@
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="B219" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="C219" t="s">
         <v>536</v>
@@ -5970,10 +5989,10 @@
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B220" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="C220" t="s">
         <v>536</v>
@@ -5981,10 +6000,10 @@
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="B221" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="C221" t="s">
         <v>536</v>
@@ -5992,10 +6011,10 @@
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="B222" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="C222" t="s">
         <v>536</v>
@@ -6003,21 +6022,21 @@
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="B223" t="s">
-        <v>616</v>
-      </c>
-      <c r="C223" t="s">
-        <v>536</v>
+        <v>618</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B224" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>661</v>
@@ -6025,10 +6044,10 @@
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="B225" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>661</v>
@@ -6036,10 +6055,10 @@
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="B226" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>661</v>
@@ -6047,21 +6066,21 @@
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>623</v>
+        <v>920</v>
       </c>
       <c r="B227" t="s">
-        <v>624</v>
-      </c>
-      <c r="C227" s="1" t="s">
-        <v>661</v>
+        <v>921</v>
+      </c>
+      <c r="C227" t="s">
+        <v>922</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c r="B228" t="s">
-        <v>921</v>
+        <v>924</v>
       </c>
       <c r="C228" t="s">
         <v>922</v>
@@ -6069,21 +6088,21 @@
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>923</v>
+        <v>234</v>
       </c>
       <c r="B229" t="s">
-        <v>924</v>
+        <v>235</v>
       </c>
       <c r="C229" t="s">
-        <v>922</v>
+        <v>988</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B230" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C230" t="s">
         <v>988</v>
@@ -6091,10 +6110,10 @@
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B231" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C231" t="s">
         <v>988</v>
@@ -6102,10 +6121,10 @@
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B232" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C232" t="s">
         <v>988</v>
@@ -6113,10 +6132,10 @@
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B233" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C233" t="s">
         <v>988</v>
@@ -6124,10 +6143,10 @@
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B234" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C234" t="s">
         <v>988</v>
@@ -6135,10 +6154,10 @@
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B235" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C235" t="s">
         <v>988</v>
@@ -6146,10 +6165,10 @@
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B236" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C236" t="s">
         <v>988</v>
@@ -6157,10 +6176,10 @@
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B237" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C237" t="s">
         <v>988</v>
@@ -6168,10 +6187,10 @@
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B238" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C238" t="s">
         <v>988</v>
@@ -6179,10 +6198,10 @@
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B239" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C239" t="s">
         <v>988</v>
@@ -6190,10 +6209,10 @@
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B240" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C240" t="s">
         <v>988</v>
@@ -6201,10 +6220,10 @@
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B241" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C241" t="s">
         <v>988</v>
@@ -6212,10 +6231,10 @@
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B242" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C242" t="s">
         <v>988</v>
@@ -6223,10 +6242,10 @@
     </row>
     <row r="243" spans="1:3">
       <c r="A243" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B243" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C243" t="s">
         <v>988</v>
@@ -6234,10 +6253,10 @@
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B244" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C244" t="s">
         <v>988</v>
@@ -6245,10 +6264,10 @@
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B245" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C245" t="s">
         <v>988</v>
@@ -6256,10 +6275,10 @@
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B246" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C246" t="s">
         <v>988</v>
@@ -6267,10 +6286,10 @@
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B247" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C247" t="s">
         <v>988</v>
@@ -6278,10 +6297,10 @@
     </row>
     <row r="248" spans="1:3">
       <c r="A248" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B248" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C248" t="s">
         <v>988</v>
@@ -6289,10 +6308,10 @@
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B249" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C249" t="s">
         <v>988</v>
@@ -6300,10 +6319,10 @@
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B250" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C250" t="s">
         <v>988</v>
@@ -6311,10 +6330,10 @@
     </row>
     <row r="251" spans="1:3">
       <c r="A251" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B251" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C251" t="s">
         <v>988</v>
@@ -6322,10 +6341,10 @@
     </row>
     <row r="252" spans="1:3">
       <c r="A252" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B252" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C252" t="s">
         <v>988</v>
@@ -6333,10 +6352,10 @@
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B253" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C253" t="s">
         <v>988</v>
@@ -6344,10 +6363,10 @@
     </row>
     <row r="254" spans="1:3">
       <c r="A254" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B254" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C254" t="s">
         <v>988</v>
@@ -6355,10 +6374,10 @@
     </row>
     <row r="255" spans="1:3">
       <c r="A255" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B255" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C255" t="s">
         <v>988</v>
@@ -6366,10 +6385,10 @@
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B256" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C256" t="s">
         <v>988</v>
@@ -6377,10 +6396,10 @@
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B257" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C257" t="s">
         <v>988</v>
@@ -6388,10 +6407,10 @@
     </row>
     <row r="258" spans="1:3">
       <c r="A258" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B258" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C258" t="s">
         <v>988</v>
@@ -6399,10 +6418,10 @@
     </row>
     <row r="259" spans="1:3">
       <c r="A259" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B259" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C259" t="s">
         <v>988</v>
@@ -6410,10 +6429,10 @@
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B260" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C260" t="s">
         <v>988</v>
@@ -6421,12 +6440,12 @@
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>296</v>
+        <v>1057</v>
       </c>
       <c r="B261" t="s">
-        <v>297</v>
-      </c>
-      <c r="C261" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C261" s="1" t="s">
         <v>988</v>
       </c>
     </row>
@@ -6927,10 +6946,10 @@
     </row>
     <row r="307" spans="1:3">
       <c r="A307" t="s">
-        <v>327</v>
+        <v>182</v>
       </c>
       <c r="B307" t="s">
-        <v>328</v>
+        <v>183</v>
       </c>
       <c r="C307" t="s">
         <v>329</v>
@@ -6938,10 +6957,10 @@
     </row>
     <row r="308" spans="1:3">
       <c r="A308" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B308" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C308" t="s">
         <v>329</v>
@@ -6949,10 +6968,10 @@
     </row>
     <row r="309" spans="1:3">
       <c r="A309" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B309" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C309" t="s">
         <v>329</v>
@@ -6960,10 +6979,10 @@
     </row>
     <row r="310" spans="1:3">
       <c r="A310" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B310" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C310" t="s">
         <v>329</v>
@@ -6971,10 +6990,10 @@
     </row>
     <row r="311" spans="1:3">
       <c r="A311" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B311" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C311" t="s">
         <v>329</v>
@@ -6982,10 +7001,10 @@
     </row>
     <row r="312" spans="1:3">
       <c r="A312" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B312" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C312" t="s">
         <v>329</v>
@@ -6993,10 +7012,10 @@
     </row>
     <row r="313" spans="1:3">
       <c r="A313" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B313" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C313" t="s">
         <v>329</v>
@@ -7004,10 +7023,10 @@
     </row>
     <row r="314" spans="1:3">
       <c r="A314" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B314" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C314" t="s">
         <v>329</v>
@@ -7015,10 +7034,10 @@
     </row>
     <row r="315" spans="1:3">
       <c r="A315" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B315" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C315" t="s">
         <v>329</v>
@@ -7026,10 +7045,10 @@
     </row>
     <row r="316" spans="1:3">
       <c r="A316" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B316" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C316" t="s">
         <v>329</v>
@@ -7037,10 +7056,10 @@
     </row>
     <row r="317" spans="1:3">
       <c r="A317" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B317" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C317" t="s">
         <v>329</v>
@@ -7048,10 +7067,10 @@
     </row>
     <row r="318" spans="1:3">
       <c r="A318" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B318" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C318" t="s">
         <v>329</v>
@@ -7059,10 +7078,10 @@
     </row>
     <row r="319" spans="1:3">
       <c r="A319" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B319" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C319" t="s">
         <v>329</v>
@@ -7070,10 +7089,10 @@
     </row>
     <row r="320" spans="1:3">
       <c r="A320" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B320" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C320" t="s">
         <v>329</v>
@@ -7081,10 +7100,10 @@
     </row>
     <row r="321" spans="1:3">
       <c r="A321" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B321" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C321" t="s">
         <v>329</v>
@@ -7092,10 +7111,10 @@
     </row>
     <row r="322" spans="1:3">
       <c r="A322" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B322" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C322" t="s">
         <v>329</v>
@@ -7103,21 +7122,21 @@
     </row>
     <row r="323" spans="1:3">
       <c r="A323" t="s">
-        <v>932</v>
+        <v>358</v>
       </c>
       <c r="B323" t="s">
-        <v>933</v>
+        <v>359</v>
       </c>
       <c r="C323" t="s">
-        <v>934</v>
+        <v>329</v>
       </c>
     </row>
     <row r="324" spans="1:3">
       <c r="A324" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="B324" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="C324" t="s">
         <v>934</v>
@@ -7125,21 +7144,21 @@
     </row>
     <row r="325" spans="1:3">
       <c r="A325" t="s">
-        <v>760</v>
+        <v>935</v>
       </c>
       <c r="B325" t="s">
-        <v>761</v>
+        <v>936</v>
       </c>
       <c r="C325" t="s">
-        <v>762</v>
+        <v>934</v>
       </c>
     </row>
     <row r="326" spans="1:3">
       <c r="A326" t="s">
-        <v>989</v>
+        <v>760</v>
       </c>
       <c r="B326" t="s">
-        <v>990</v>
+        <v>761</v>
       </c>
       <c r="C326" t="s">
         <v>762</v>
@@ -7147,10 +7166,10 @@
     </row>
     <row r="327" spans="1:3">
       <c r="A327" t="s">
-        <v>763</v>
+        <v>989</v>
       </c>
       <c r="B327" t="s">
-        <v>764</v>
+        <v>990</v>
       </c>
       <c r="C327" t="s">
         <v>762</v>
@@ -7158,10 +7177,10 @@
     </row>
     <row r="328" spans="1:3">
       <c r="A328" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B328" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C328" t="s">
         <v>762</v>
@@ -7169,10 +7188,10 @@
     </row>
     <row r="329" spans="1:3">
       <c r="A329" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B329" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C329" t="s">
         <v>762</v>
@@ -7180,10 +7199,10 @@
     </row>
     <row r="330" spans="1:3">
       <c r="A330" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="B330" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C330" t="s">
         <v>762</v>
@@ -7191,21 +7210,21 @@
     </row>
     <row r="331" spans="1:3">
       <c r="A331" t="s">
-        <v>937</v>
+        <v>769</v>
       </c>
       <c r="B331" t="s">
-        <v>938</v>
+        <v>770</v>
       </c>
       <c r="C331" t="s">
-        <v>939</v>
+        <v>762</v>
       </c>
     </row>
     <row r="332" spans="1:3">
       <c r="A332" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="B332" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="C332" t="s">
         <v>939</v>
@@ -7213,10 +7232,10 @@
     </row>
     <row r="333" spans="1:3">
       <c r="A333" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="B333" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C333" t="s">
         <v>939</v>
@@ -7224,10 +7243,10 @@
     </row>
     <row r="334" spans="1:3">
       <c r="A334" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="B334" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="C334" t="s">
         <v>939</v>
@@ -7235,10 +7254,10 @@
     </row>
     <row r="335" spans="1:3">
       <c r="A335" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="B335" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="C335" t="s">
         <v>939</v>
@@ -7246,10 +7265,10 @@
     </row>
     <row r="336" spans="1:3">
       <c r="A336" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="B336" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="C336" t="s">
         <v>939</v>
@@ -7257,10 +7276,10 @@
     </row>
     <row r="337" spans="1:3">
       <c r="A337" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="B337" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="C337" t="s">
         <v>939</v>
@@ -7268,21 +7287,21 @@
     </row>
     <row r="338" spans="1:3">
       <c r="A338" t="s">
-        <v>298</v>
+        <v>950</v>
       </c>
       <c r="B338" t="s">
-        <v>299</v>
+        <v>951</v>
       </c>
       <c r="C338" t="s">
-        <v>991</v>
+        <v>939</v>
       </c>
     </row>
     <row r="339" spans="1:3">
       <c r="A339" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B339" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C339" t="s">
         <v>991</v>
@@ -7290,10 +7309,10 @@
     </row>
     <row r="340" spans="1:3">
       <c r="A340" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B340" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C340" t="s">
         <v>991</v>
@@ -7301,10 +7320,10 @@
     </row>
     <row r="341" spans="1:3">
       <c r="A341" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B341" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C341" t="s">
         <v>991</v>
@@ -7312,10 +7331,10 @@
     </row>
     <row r="342" spans="1:3">
       <c r="A342" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B342" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C342" t="s">
         <v>991</v>
@@ -7323,10 +7342,10 @@
     </row>
     <row r="343" spans="1:3">
       <c r="A343" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B343" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C343" t="s">
         <v>991</v>
@@ -7334,10 +7353,10 @@
     </row>
     <row r="344" spans="1:3">
       <c r="A344" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B344" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C344" t="s">
         <v>991</v>
@@ -7345,10 +7364,10 @@
     </row>
     <row r="345" spans="1:3">
       <c r="A345" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B345" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C345" t="s">
         <v>991</v>
@@ -7356,10 +7375,10 @@
     </row>
     <row r="346" spans="1:3">
       <c r="A346" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B346" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C346" t="s">
         <v>991</v>
@@ -7367,21 +7386,21 @@
     </row>
     <row r="347" spans="1:3">
       <c r="A347" t="s">
-        <v>954</v>
+        <v>314</v>
       </c>
       <c r="B347" t="s">
-        <v>955</v>
+        <v>315</v>
       </c>
       <c r="C347" t="s">
-        <v>956</v>
+        <v>991</v>
       </c>
     </row>
     <row r="348" spans="1:3">
       <c r="A348" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="B348" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="C348" t="s">
         <v>956</v>
@@ -7389,10 +7408,10 @@
     </row>
     <row r="349" spans="1:3">
       <c r="A349" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="B349" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C349" t="s">
         <v>956</v>
@@ -7400,10 +7419,10 @@
     </row>
     <row r="350" spans="1:3">
       <c r="A350" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="B350" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C350" t="s">
         <v>956</v>
@@ -7411,10 +7430,10 @@
     </row>
     <row r="351" spans="1:3">
       <c r="A351" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B351" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="C351" t="s">
         <v>956</v>
@@ -7422,10 +7441,10 @@
     </row>
     <row r="352" spans="1:3">
       <c r="A352" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="B352" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="C352" t="s">
         <v>956</v>
@@ -7433,21 +7452,21 @@
     </row>
     <row r="353" spans="1:3">
       <c r="A353" t="s">
-        <v>360</v>
+        <v>965</v>
       </c>
       <c r="B353" t="s">
-        <v>361</v>
+        <v>966</v>
       </c>
       <c r="C353" t="s">
-        <v>362</v>
+        <v>956</v>
       </c>
     </row>
     <row r="354" spans="1:3">
       <c r="A354" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B354" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C354" t="s">
         <v>362</v>
@@ -7455,10 +7474,10 @@
     </row>
     <row r="355" spans="1:3">
       <c r="A355" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B355" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C355" t="s">
         <v>362</v>
@@ -7466,10 +7485,10 @@
     </row>
     <row r="356" spans="1:3">
       <c r="A356" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B356" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C356" t="s">
         <v>362</v>
@@ -7477,10 +7496,10 @@
     </row>
     <row r="357" spans="1:3">
       <c r="A357" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B357" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C357" t="s">
         <v>362</v>
@@ -7488,10 +7507,10 @@
     </row>
     <row r="358" spans="1:3">
       <c r="A358" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B358" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C358" t="s">
         <v>362</v>
@@ -7499,10 +7518,10 @@
     </row>
     <row r="359" spans="1:3">
       <c r="A359" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B359" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C359" t="s">
         <v>362</v>
@@ -7510,10 +7529,10 @@
     </row>
     <row r="360" spans="1:3">
       <c r="A360" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B360" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C360" t="s">
         <v>362</v>
@@ -7521,21 +7540,21 @@
     </row>
     <row r="361" spans="1:3">
       <c r="A361" t="s">
-        <v>992</v>
+        <v>375</v>
       </c>
       <c r="B361" t="s">
-        <v>993</v>
+        <v>376</v>
       </c>
       <c r="C361" t="s">
-        <v>994</v>
+        <v>362</v>
       </c>
     </row>
     <row r="362" spans="1:3">
       <c r="A362" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="B362" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="C362" t="s">
         <v>994</v>
@@ -7543,21 +7562,21 @@
     </row>
     <row r="363" spans="1:3">
       <c r="A363" t="s">
-        <v>816</v>
+        <v>995</v>
       </c>
       <c r="B363" t="s">
-        <v>817</v>
+        <v>996</v>
       </c>
       <c r="C363" t="s">
-        <v>818</v>
+        <v>994</v>
       </c>
     </row>
     <row r="364" spans="1:3">
       <c r="A364" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="B364" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="C364" t="s">
         <v>818</v>
@@ -7565,10 +7584,10 @@
     </row>
     <row r="365" spans="1:3">
       <c r="A365" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B365" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C365" t="s">
         <v>818</v>
@@ -7576,10 +7595,10 @@
     </row>
     <row r="366" spans="1:3">
       <c r="A366" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B366" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="C366" t="s">
         <v>818</v>
@@ -7587,10 +7606,10 @@
     </row>
     <row r="367" spans="1:3">
       <c r="A367" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B367" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="C367" t="s">
         <v>818</v>
@@ -7598,10 +7617,10 @@
     </row>
     <row r="368" spans="1:3">
       <c r="A368" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B368" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="C368" t="s">
         <v>818</v>
@@ -7609,10 +7628,10 @@
     </row>
     <row r="369" spans="1:3">
       <c r="A369" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B369" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C369" t="s">
         <v>818</v>
@@ -7620,10 +7639,10 @@
     </row>
     <row r="370" spans="1:3">
       <c r="A370" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B370" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C370" t="s">
         <v>818</v>
@@ -7631,10 +7650,10 @@
     </row>
     <row r="371" spans="1:3">
       <c r="A371" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B371" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="C371" t="s">
         <v>818</v>
@@ -7642,10 +7661,10 @@
     </row>
     <row r="372" spans="1:3">
       <c r="A372" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B372" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="C372" t="s">
         <v>818</v>
@@ -7653,21 +7672,21 @@
     </row>
     <row r="373" spans="1:3">
       <c r="A373" t="s">
-        <v>997</v>
+        <v>835</v>
       </c>
       <c r="B373" t="s">
-        <v>998</v>
+        <v>836</v>
       </c>
       <c r="C373" t="s">
-        <v>999</v>
+        <v>818</v>
       </c>
     </row>
     <row r="374" spans="1:3">
       <c r="A374" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="B374" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="C374" t="s">
         <v>999</v>
@@ -7675,10 +7694,10 @@
     </row>
     <row r="375" spans="1:3">
       <c r="A375" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="B375" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C375" t="s">
         <v>999</v>
@@ -7686,21 +7705,21 @@
     </row>
     <row r="376" spans="1:3">
       <c r="A376" t="s">
-        <v>377</v>
+        <v>1002</v>
       </c>
       <c r="B376" t="s">
-        <v>378</v>
+        <v>1003</v>
       </c>
       <c r="C376" t="s">
-        <v>1004</v>
+        <v>999</v>
       </c>
     </row>
     <row r="377" spans="1:3">
       <c r="A377" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B377" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C377" t="s">
         <v>1004</v>
@@ -7708,10 +7727,10 @@
     </row>
     <row r="378" spans="1:3">
       <c r="A378" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B378" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C378" t="s">
         <v>1004</v>
@@ -7719,10 +7738,10 @@
     </row>
     <row r="379" spans="1:3">
       <c r="A379" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B379" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C379" t="s">
         <v>1004</v>
@@ -7730,10 +7749,10 @@
     </row>
     <row r="380" spans="1:3">
       <c r="A380" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B380" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C380" t="s">
         <v>1004</v>
@@ -7741,10 +7760,10 @@
     </row>
     <row r="381" spans="1:3">
       <c r="A381" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B381" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C381" t="s">
         <v>1004</v>
@@ -7752,10 +7771,10 @@
     </row>
     <row r="382" spans="1:3">
       <c r="A382" t="s">
-        <v>1005</v>
+        <v>387</v>
       </c>
       <c r="B382" t="s">
-        <v>1006</v>
+        <v>388</v>
       </c>
       <c r="C382" t="s">
         <v>1004</v>
@@ -7763,10 +7782,10 @@
     </row>
     <row r="383" spans="1:3">
       <c r="A383" t="s">
-        <v>389</v>
+        <v>1005</v>
       </c>
       <c r="B383" t="s">
-        <v>390</v>
+        <v>1006</v>
       </c>
       <c r="C383" t="s">
         <v>1004</v>
@@ -7774,10 +7793,10 @@
     </row>
     <row r="384" spans="1:3">
       <c r="A384" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B384" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C384" t="s">
         <v>1004</v>
@@ -7785,10 +7804,10 @@
     </row>
     <row r="385" spans="1:3">
       <c r="A385" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B385" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C385" t="s">
         <v>1004</v>
@@ -7796,10 +7815,10 @@
     </row>
     <row r="386" spans="1:3">
       <c r="A386" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B386" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C386" t="s">
         <v>1004</v>
@@ -7807,10 +7826,10 @@
     </row>
     <row r="387" spans="1:3">
       <c r="A387" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B387" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C387" t="s">
         <v>1004</v>
@@ -7818,10 +7837,10 @@
     </row>
     <row r="388" spans="1:3">
       <c r="A388" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B388" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C388" t="s">
         <v>1004</v>
@@ -7829,21 +7848,21 @@
     </row>
     <row r="389" spans="1:3">
       <c r="A389" t="s">
-        <v>635</v>
+        <v>399</v>
       </c>
       <c r="B389" t="s">
-        <v>636</v>
+        <v>400</v>
       </c>
       <c r="C389" t="s">
-        <v>637</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="390" spans="1:3">
       <c r="A390" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="B390" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C390" t="s">
         <v>637</v>
@@ -7851,10 +7870,10 @@
     </row>
     <row r="391" spans="1:3">
       <c r="A391" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B391" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C391" t="s">
         <v>637</v>
@@ -7862,10 +7881,10 @@
     </row>
     <row r="392" spans="1:3">
       <c r="A392" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B392" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C392" t="s">
         <v>637</v>
@@ -7873,10 +7892,10 @@
     </row>
     <row r="393" spans="1:3">
       <c r="A393" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B393" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C393" t="s">
         <v>637</v>
@@ -7884,10 +7903,10 @@
     </row>
     <row r="394" spans="1:3">
       <c r="A394" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B394" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C394" t="s">
         <v>637</v>
@@ -7895,21 +7914,21 @@
     </row>
     <row r="395" spans="1:3">
       <c r="A395" t="s">
-        <v>837</v>
+        <v>646</v>
       </c>
       <c r="B395" t="s">
-        <v>838</v>
+        <v>647</v>
       </c>
       <c r="C395" t="s">
-        <v>839</v>
+        <v>637</v>
       </c>
     </row>
     <row r="396" spans="1:3">
       <c r="A396" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="B396" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C396" t="s">
         <v>839</v>
@@ -7917,10 +7936,10 @@
     </row>
     <row r="397" spans="1:3">
       <c r="A397" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B397" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="C397" t="s">
         <v>839</v>
@@ -7928,10 +7947,10 @@
     </row>
     <row r="398" spans="1:3">
       <c r="A398" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="B398" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C398" t="s">
         <v>839</v>
@@ -7939,10 +7958,10 @@
     </row>
     <row r="399" spans="1:3">
       <c r="A399" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B399" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C399" t="s">
         <v>839</v>
@@ -7950,10 +7969,10 @@
     </row>
     <row r="400" spans="1:3">
       <c r="A400" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B400" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C400" t="s">
         <v>839</v>
@@ -7961,10 +7980,10 @@
     </row>
     <row r="401" spans="1:3">
       <c r="A401" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="B401" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="C401" t="s">
         <v>839</v>
@@ -7972,10 +7991,10 @@
     </row>
     <row r="402" spans="1:3">
       <c r="A402" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B402" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="C402" t="s">
         <v>839</v>
@@ -7983,10 +8002,10 @@
     </row>
     <row r="403" spans="1:3">
       <c r="A403" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="B403" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C403" t="s">
         <v>839</v>
@@ -7994,10 +8013,10 @@
     </row>
     <row r="404" spans="1:3">
       <c r="A404" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="B404" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="C404" t="s">
         <v>839</v>
@@ -8005,10 +8024,10 @@
     </row>
     <row r="405" spans="1:3">
       <c r="A405" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="B405" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="C405" t="s">
         <v>839</v>
@@ -8016,10 +8035,10 @@
     </row>
     <row r="406" spans="1:3">
       <c r="A406" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B406" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="C406" t="s">
         <v>839</v>
@@ -8027,21 +8046,21 @@
     </row>
     <row r="407" spans="1:3">
       <c r="A407" t="s">
-        <v>1007</v>
+        <v>860</v>
       </c>
       <c r="B407" t="s">
-        <v>1008</v>
+        <v>861</v>
       </c>
       <c r="C407" t="s">
-        <v>1009</v>
+        <v>839</v>
       </c>
     </row>
     <row r="408" spans="1:3">
       <c r="A408" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="B408" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="C408" t="s">
         <v>1009</v>
@@ -8049,21 +8068,21 @@
     </row>
     <row r="409" spans="1:3">
       <c r="A409" t="s">
-        <v>663</v>
+        <v>1010</v>
       </c>
       <c r="B409" t="s">
-        <v>664</v>
+        <v>1011</v>
       </c>
       <c r="C409" t="s">
-        <v>665</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="410" spans="1:3">
       <c r="A410" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="B410" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="C410" t="s">
         <v>665</v>
@@ -8071,10 +8090,10 @@
     </row>
     <row r="411" spans="1:3">
       <c r="A411" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B411" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C411" t="s">
         <v>665</v>
@@ -8082,10 +8101,10 @@
     </row>
     <row r="412" spans="1:3">
       <c r="A412" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B412" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C412" t="s">
         <v>665</v>
@@ -8093,21 +8112,21 @@
     </row>
     <row r="413" spans="1:3">
       <c r="A413" t="s">
-        <v>648</v>
+        <v>670</v>
       </c>
       <c r="B413" t="s">
-        <v>649</v>
+        <v>671</v>
       </c>
       <c r="C413" t="s">
-        <v>650</v>
+        <v>665</v>
       </c>
     </row>
     <row r="414" spans="1:3">
       <c r="A414" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="B414" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C414" t="s">
         <v>650</v>
@@ -8115,10 +8134,10 @@
     </row>
     <row r="415" spans="1:3">
       <c r="A415" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B415" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C415" t="s">
         <v>650</v>
@@ -8126,10 +8145,10 @@
     </row>
     <row r="416" spans="1:3">
       <c r="A416" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B416" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C416" t="s">
         <v>650</v>
@@ -8137,10 +8156,10 @@
     </row>
     <row r="417" spans="1:3">
       <c r="A417" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B417" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C417" t="s">
         <v>650</v>
@@ -8148,10 +8167,10 @@
     </row>
     <row r="418" spans="1:3">
       <c r="A418" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B418" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C418" t="s">
         <v>650</v>
@@ -8159,21 +8178,21 @@
     </row>
     <row r="419" spans="1:3">
       <c r="A419" t="s">
-        <v>1012</v>
+        <v>659</v>
       </c>
       <c r="B419" t="s">
-        <v>1013</v>
+        <v>660</v>
       </c>
       <c r="C419" t="s">
-        <v>1014</v>
+        <v>650</v>
       </c>
     </row>
     <row r="420" spans="1:3">
       <c r="A420" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="B420" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="C420" t="s">
         <v>1014</v>
@@ -8181,10 +8200,10 @@
     </row>
     <row r="421" spans="1:3">
       <c r="A421" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="B421" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="C421" t="s">
         <v>1014</v>
@@ -8192,10 +8211,10 @@
     </row>
     <row r="422" spans="1:3">
       <c r="A422" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="B422" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="C422" t="s">
         <v>1014</v>
@@ -8203,21 +8222,21 @@
     </row>
     <row r="423" spans="1:3">
       <c r="A423" t="s">
-        <v>672</v>
+        <v>1019</v>
       </c>
       <c r="B423" t="s">
-        <v>673</v>
+        <v>1020</v>
       </c>
       <c r="C423" t="s">
-        <v>674</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="424" spans="1:3">
       <c r="A424" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="B424" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="C424" t="s">
         <v>674</v>
@@ -8225,10 +8244,10 @@
     </row>
     <row r="425" spans="1:3">
       <c r="A425" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B425" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C425" t="s">
         <v>674</v>
@@ -8236,10 +8255,10 @@
     </row>
     <row r="426" spans="1:3">
       <c r="A426" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B426" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C426" t="s">
         <v>674</v>
@@ -8247,21 +8266,21 @@
     </row>
     <row r="427" spans="1:3">
       <c r="A427" t="s">
-        <v>433</v>
+        <v>679</v>
       </c>
       <c r="B427" t="s">
-        <v>401</v>
+        <v>680</v>
       </c>
       <c r="C427" t="s">
-        <v>402</v>
+        <v>674</v>
       </c>
     </row>
     <row r="428" spans="1:3">
       <c r="A428" t="s">
-        <v>403</v>
+        <v>433</v>
       </c>
       <c r="B428" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C428" t="s">
         <v>402</v>
@@ -8269,10 +8288,10 @@
     </row>
     <row r="429" spans="1:3">
       <c r="A429" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B429" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C429" t="s">
         <v>402</v>
@@ -8280,10 +8299,10 @@
     </row>
     <row r="430" spans="1:3">
       <c r="A430" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B430" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C430" t="s">
         <v>402</v>
@@ -8291,10 +8310,10 @@
     </row>
     <row r="431" spans="1:3">
       <c r="A431" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B431" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C431" t="s">
         <v>402</v>
@@ -8302,10 +8321,10 @@
     </row>
     <row r="432" spans="1:3">
       <c r="A432" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B432" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C432" t="s">
         <v>402</v>
@@ -8313,10 +8332,10 @@
     </row>
     <row r="433" spans="1:3">
       <c r="A433" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B433" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C433" t="s">
         <v>402</v>
@@ -8324,10 +8343,10 @@
     </row>
     <row r="434" spans="1:3">
       <c r="A434" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B434" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C434" t="s">
         <v>402</v>
@@ -8335,10 +8354,10 @@
     </row>
     <row r="435" spans="1:3">
       <c r="A435" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B435" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C435" t="s">
         <v>402</v>
@@ -8346,10 +8365,10 @@
     </row>
     <row r="436" spans="1:3">
       <c r="A436" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B436" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C436" t="s">
         <v>402</v>
@@ -8357,10 +8376,10 @@
     </row>
     <row r="437" spans="1:3">
       <c r="A437" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B437" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C437" t="s">
         <v>402</v>
@@ -8368,10 +8387,10 @@
     </row>
     <row r="438" spans="1:3">
       <c r="A438" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B438" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C438" t="s">
         <v>402</v>
@@ -8379,10 +8398,10 @@
     </row>
     <row r="439" spans="1:3">
       <c r="A439" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B439" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C439" t="s">
         <v>402</v>
@@ -8390,10 +8409,10 @@
     </row>
     <row r="440" spans="1:3">
       <c r="A440" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B440" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C440" t="s">
         <v>402</v>
@@ -8401,10 +8420,10 @@
     </row>
     <row r="441" spans="1:3">
       <c r="A441" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B441" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C441" t="s">
         <v>402</v>
@@ -8412,10 +8431,10 @@
     </row>
     <row r="442" spans="1:3">
       <c r="A442" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B442" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C442" t="s">
         <v>402</v>
@@ -8423,21 +8442,21 @@
     </row>
     <row r="443" spans="1:3">
       <c r="A443" t="s">
-        <v>681</v>
+        <v>431</v>
       </c>
       <c r="B443" t="s">
-        <v>682</v>
+        <v>432</v>
       </c>
       <c r="C443" t="s">
-        <v>1021</v>
+        <v>402</v>
       </c>
     </row>
     <row r="444" spans="1:3">
       <c r="A444" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B444" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C444" t="s">
         <v>1021</v>
@@ -8445,10 +8464,10 @@
     </row>
     <row r="445" spans="1:3">
       <c r="A445" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B445" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C445" t="s">
         <v>1021</v>
@@ -8456,10 +8475,10 @@
     </row>
     <row r="446" spans="1:3">
       <c r="A446" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B446" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C446" t="s">
         <v>1021</v>
@@ -8467,10 +8486,10 @@
     </row>
     <row r="447" spans="1:3">
       <c r="A447" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B447" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C447" t="s">
         <v>1021</v>
@@ -8478,10 +8497,10 @@
     </row>
     <row r="448" spans="1:3">
       <c r="A448" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B448" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C448" t="s">
         <v>1021</v>
@@ -8489,10 +8508,10 @@
     </row>
     <row r="449" spans="1:3">
       <c r="A449" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B449" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C449" t="s">
         <v>1021</v>
@@ -8500,10 +8519,10 @@
     </row>
     <row r="450" spans="1:3">
       <c r="A450" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B450" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C450" t="s">
         <v>1021</v>
@@ -8511,10 +8530,10 @@
     </row>
     <row r="451" spans="1:3">
       <c r="A451" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B451" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C451" t="s">
         <v>1021</v>
@@ -8522,10 +8541,10 @@
     </row>
     <row r="452" spans="1:3">
       <c r="A452" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B452" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C452" t="s">
         <v>1021</v>
@@ -8533,10 +8552,10 @@
     </row>
     <row r="453" spans="1:3">
       <c r="A453" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B453" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C453" t="s">
         <v>1021</v>
@@ -8544,10 +8563,10 @@
     </row>
     <row r="454" spans="1:3">
       <c r="A454" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B454" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C454" t="s">
         <v>1021</v>
@@ -8555,10 +8574,10 @@
     </row>
     <row r="455" spans="1:3">
       <c r="A455" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B455" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C455" t="s">
         <v>1021</v>
@@ -8566,10 +8585,10 @@
     </row>
     <row r="456" spans="1:3">
       <c r="A456" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B456" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C456" t="s">
         <v>1021</v>
@@ -8577,10 +8596,10 @@
     </row>
     <row r="457" spans="1:3">
       <c r="A457" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B457" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C457" t="s">
         <v>1021</v>
@@ -8588,10 +8607,10 @@
     </row>
     <row r="458" spans="1:3">
       <c r="A458" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B458" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C458" t="s">
         <v>1021</v>
@@ -8599,10 +8618,10 @@
     </row>
     <row r="459" spans="1:3">
       <c r="A459" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B459" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="C459" t="s">
         <v>1021</v>
@@ -8610,10 +8629,10 @@
     </row>
     <row r="460" spans="1:3">
       <c r="A460" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B460" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="C460" t="s">
         <v>1021</v>
@@ -8621,10 +8640,10 @@
     </row>
     <row r="461" spans="1:3">
       <c r="A461" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B461" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="C461" t="s">
         <v>1021</v>
@@ -8632,10 +8651,10 @@
     </row>
     <row r="462" spans="1:3">
       <c r="A462" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B462" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C462" t="s">
         <v>1021</v>
@@ -8643,10 +8662,10 @@
     </row>
     <row r="463" spans="1:3">
       <c r="A463" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B463" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C463" t="s">
         <v>1021</v>
@@ -8654,10 +8673,10 @@
     </row>
     <row r="464" spans="1:3">
       <c r="A464" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B464" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C464" t="s">
         <v>1021</v>
@@ -8665,10 +8684,10 @@
     </row>
     <row r="465" spans="1:3">
       <c r="A465" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B465" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C465" t="s">
         <v>1021</v>
@@ -8676,10 +8695,10 @@
     </row>
     <row r="466" spans="1:3">
       <c r="A466" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B466" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C466" t="s">
         <v>1021</v>
@@ -8687,10 +8706,10 @@
     </row>
     <row r="467" spans="1:3">
       <c r="A467" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B467" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C467" t="s">
         <v>1021</v>
@@ -8698,21 +8717,21 @@
     </row>
     <row r="468" spans="1:3">
       <c r="A468" t="s">
-        <v>862</v>
+        <v>729</v>
       </c>
       <c r="B468" t="s">
-        <v>863</v>
+        <v>730</v>
       </c>
       <c r="C468" t="s">
-        <v>864</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="469" spans="1:3">
       <c r="A469" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="B469" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C469" t="s">
         <v>864</v>
@@ -8720,10 +8739,10 @@
     </row>
     <row r="470" spans="1:3">
       <c r="A470" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="B470" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="C470" t="s">
         <v>864</v>
@@ -8731,10 +8750,10 @@
     </row>
     <row r="471" spans="1:3">
       <c r="A471" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B471" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="C471" t="s">
         <v>864</v>
@@ -8742,10 +8761,10 @@
     </row>
     <row r="472" spans="1:3">
       <c r="A472" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B472" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C472" t="s">
         <v>864</v>
@@ -8753,10 +8772,10 @@
     </row>
     <row r="473" spans="1:3">
       <c r="A473" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="B473" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="C473" t="s">
         <v>864</v>
@@ -8764,10 +8783,10 @@
     </row>
     <row r="474" spans="1:3">
       <c r="A474" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B474" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="C474" t="s">
         <v>864</v>
@@ -8775,10 +8794,10 @@
     </row>
     <row r="475" spans="1:3">
       <c r="A475" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B475" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="C475" t="s">
         <v>864</v>
@@ -8786,10 +8805,10 @@
     </row>
     <row r="476" spans="1:3">
       <c r="A476" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="B476" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="C476" t="s">
         <v>864</v>
@@ -8797,10 +8816,10 @@
     </row>
     <row r="477" spans="1:3">
       <c r="A477" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="B477" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="C477" t="s">
         <v>864</v>
@@ -8808,10 +8827,10 @@
     </row>
     <row r="478" spans="1:3">
       <c r="A478" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B478" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="C478" t="s">
         <v>864</v>
@@ -8819,10 +8838,10 @@
     </row>
     <row r="479" spans="1:3">
       <c r="A479" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B479" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="C479" t="s">
         <v>864</v>
@@ -8830,10 +8849,10 @@
     </row>
     <row r="480" spans="1:3">
       <c r="A480" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="B480" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="C480" t="s">
         <v>864</v>
@@ -8841,10 +8860,10 @@
     </row>
     <row r="481" spans="1:3">
       <c r="A481" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B481" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="C481" t="s">
         <v>864</v>
@@ -8852,10 +8871,10 @@
     </row>
     <row r="482" spans="1:3">
       <c r="A482" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="B482" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C482" t="s">
         <v>864</v>
@@ -8863,10 +8882,10 @@
     </row>
     <row r="483" spans="1:3">
       <c r="A483" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="B483" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="C483" t="s">
         <v>864</v>
@@ -8874,21 +8893,21 @@
     </row>
     <row r="484" spans="1:3">
       <c r="A484" t="s">
-        <v>625</v>
+        <v>893</v>
       </c>
       <c r="B484" t="s">
-        <v>626</v>
+        <v>894</v>
       </c>
       <c r="C484" t="s">
-        <v>1022</v>
+        <v>864</v>
       </c>
     </row>
     <row r="485" spans="1:3">
       <c r="A485" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B485" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C485" t="s">
         <v>1022</v>
@@ -8896,10 +8915,10 @@
     </row>
     <row r="486" spans="1:3">
       <c r="A486" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B486" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C486" t="s">
         <v>1022</v>
@@ -8907,10 +8926,10 @@
     </row>
     <row r="487" spans="1:3">
       <c r="A487" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B487" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C487" t="s">
         <v>1022</v>
@@ -8918,10 +8937,10 @@
     </row>
     <row r="488" spans="1:3">
       <c r="A488" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B488" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C488" t="s">
         <v>1022</v>
@@ -8929,21 +8948,21 @@
     </row>
     <row r="489" spans="1:3">
       <c r="A489" t="s">
-        <v>1023</v>
+        <v>633</v>
       </c>
       <c r="B489" t="s">
-        <v>1024</v>
+        <v>634</v>
       </c>
       <c r="C489" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="490" spans="1:3">
       <c r="A490" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="B490" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="C490" t="s">
         <v>1025</v>
@@ -8951,10 +8970,10 @@
     </row>
     <row r="491" spans="1:3">
       <c r="A491" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="B491" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="C491" t="s">
         <v>1025</v>
@@ -8962,10 +8981,10 @@
     </row>
     <row r="492" spans="1:3">
       <c r="A492" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="B492" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="C492" t="s">
         <v>1025</v>
@@ -8973,10 +8992,10 @@
     </row>
     <row r="493" spans="1:3">
       <c r="A493" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="B493" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="C493" t="s">
         <v>1025</v>
@@ -8984,10 +9003,10 @@
     </row>
     <row r="494" spans="1:3">
       <c r="A494" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="B494" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="C494" t="s">
         <v>1025</v>
@@ -8995,10 +9014,10 @@
     </row>
     <row r="495" spans="1:3">
       <c r="A495" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="B495" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="C495" t="s">
         <v>1025</v>
@@ -9006,10 +9025,10 @@
     </row>
     <row r="496" spans="1:3">
       <c r="A496" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B496" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="C496" t="s">
         <v>1025</v>
@@ -9017,10 +9036,10 @@
     </row>
     <row r="497" spans="1:3">
       <c r="A497" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="B497" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="C497" t="s">
         <v>1025</v>
@@ -9028,10 +9047,10 @@
     </row>
     <row r="498" spans="1:3">
       <c r="A498" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="B498" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="C498" t="s">
         <v>1025</v>
@@ -9039,10 +9058,10 @@
     </row>
     <row r="499" spans="1:3">
       <c r="A499" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="B499" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="C499" t="s">
         <v>1025</v>
@@ -9050,10 +9069,10 @@
     </row>
     <row r="500" spans="1:3">
       <c r="A500" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="B500" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="C500" t="s">
         <v>1025</v>
@@ -9061,10 +9080,10 @@
     </row>
     <row r="501" spans="1:3">
       <c r="A501" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="B501" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="C501" t="s">
         <v>1025</v>
@@ -9072,10 +9091,10 @@
     </row>
     <row r="502" spans="1:3">
       <c r="A502" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="B502" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="C502" t="s">
         <v>1025</v>
@@ -9083,10 +9102,10 @@
     </row>
     <row r="503" spans="1:3">
       <c r="A503" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="B503" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="C503" t="s">
         <v>1025</v>
@@ -9094,18 +9113,29 @@
     </row>
     <row r="504" spans="1:3">
       <c r="A504" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="B504" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="C504" t="s">
         <v>1025</v>
       </c>
     </row>
+    <row r="505" spans="1:3">
+      <c r="A505" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B505" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C505" t="s">
+        <v>1025</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C504">
-    <sortCondition ref="C1:C504"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C505">
+    <sortCondition ref="C1:C505"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>